<commit_message>
IHW: SIM docrules hersteld (nu met plaatjes e.d.)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -967,6 +967,9 @@
   </si>
   <si>
     <t>URL of the Github IO (pages) location</t>
+  </si>
+  <si>
+    <t>IHWBMS</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1114,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1222,6 +1225,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1519,10 +1525,10 @@
   <dimension ref="A1:V132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1770,16 +1776,16 @@
       <c r="V6"/>
     </row>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="42" t="b">
+      <c r="D7" s="43" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1799,10 +1805,10 @@
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -3099,16 +3105,16 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="42" t="b">
+      <c r="D44" s="43" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3131,10 +3137,10 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="17"/>
@@ -3250,24 +3256,45 @@
       <c r="E49" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="G49" s="21"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
+      <c r="H49" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="I49" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="J49" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="K49" s="42" t="s">
+        <v>290</v>
+      </c>
       <c r="L49" s="21"/>
-      <c r="M49" s="33"/>
-      <c r="N49" s="33"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
+      <c r="M49" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="N49" s="42" t="s">
+        <v>291</v>
+      </c>
+      <c r="O49" s="42" t="s">
+        <v>291</v>
+      </c>
+      <c r="P49" s="42" t="s">
+        <v>291</v>
+      </c>
       <c r="Q49" s="21"/>
-      <c r="R49" s="38"/>
-      <c r="S49" s="38"/>
-      <c r="T49" s="38"/>
-      <c r="U49" s="38"/>
+      <c r="R49" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="S49" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="T49" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="U49" s="42" t="s">
+        <v>314</v>
+      </c>
       <c r="V49"/>
     </row>
     <row r="50" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
IHW: correcties configuratie UGM
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -1114,7 +1114,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1225,6 +1225,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1525,10 +1528,10 @@
   <dimension ref="A1:V132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1776,16 +1779,16 @@
       <c r="V6"/>
     </row>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="43" t="b">
+      <c r="D7" s="44" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1805,10 +1808,10 @@
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -2684,20 +2687,45 @@
       <c r="E31" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="20"/>
+      <c r="H31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="20"/>
+      <c r="I31" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>34</v>
+      </c>
       <c r="L31" s="20"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
+      <c r="M31" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="O31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="P31" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="Q31" s="27"/>
-      <c r="R31" s="38"/>
-      <c r="S31" s="38"/>
-      <c r="T31" s="38"/>
-      <c r="U31" s="38"/>
+      <c r="R31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="S31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="T31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="U31" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="V31"/>
     </row>
     <row r="32" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3105,16 +3133,16 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="43" t="b">
+      <c r="D44" s="44" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3137,10 +3165,10 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="17"/>
@@ -3943,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G71" s="20"/>
       <c r="L71" s="20"/>

</xml_diff>

<commit_message>
IHW: correctie configuratie fout
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="314">
   <si>
     <t>Name</t>
   </si>
@@ -967,9 +967,6 @@
   </si>
   <si>
     <t>URL of the Github IO (pages) location</t>
-  </si>
-  <si>
-    <t>IHWBMS</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1111,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1225,6 +1222,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1528,10 +1528,10 @@
   <dimension ref="A1:V132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="S49" sqref="S49:U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1779,16 +1779,16 @@
       <c r="V6"/>
     </row>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="44" t="b">
+      <c r="D7" s="45" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1808,10 +1808,10 @@
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -3133,16 +3133,16 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="44" t="b">
+      <c r="D44" s="45" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3165,10 +3165,10 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="44"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="17"/>
@@ -3312,16 +3312,16 @@
       </c>
       <c r="Q49" s="21"/>
       <c r="R49" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="S49" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="T49" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="U49" s="42" t="s">
-        <v>314</v>
+        <v>292</v>
+      </c>
+      <c r="S49" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="T49" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="U49" s="44" t="s">
+        <v>292</v>
       </c>
       <c r="V49"/>
     </row>

</xml_diff>

<commit_message>
IHW: nieuwe settings voor samenstellen OpenAPI
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -967,6 +967,9 @@
   </si>
   <si>
     <t>URL of the Github IO (pages) location</t>
+  </si>
+  <si>
+    <t>NVT</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1114,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1222,6 +1225,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1528,10 +1537,10 @@
   <dimension ref="A1:V132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S49" sqref="S49:U49"/>
+      <selection pane="bottomRight" activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1779,16 +1788,16 @@
       <c r="V6"/>
     </row>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="45" t="b">
+      <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1808,10 +1817,10 @@
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -2594,45 +2603,23 @@
       <c r="E29" s="28" t="b">
         <v>1</v>
       </c>
+      <c r="F29" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="G29" s="27"/>
-      <c r="H29" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="29" t="s">
-        <v>16</v>
-      </c>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
       <c r="L29" s="27"/>
-      <c r="M29" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="O29" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="28" t="s">
-        <v>4</v>
-      </c>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
       <c r="Q29" s="27"/>
-      <c r="R29" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="S29" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="T29" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="U29" s="38" t="s">
-        <v>4</v>
-      </c>
+      <c r="R29" s="45"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="46"/>
       <c r="V29"/>
     </row>
     <row r="30" spans="1:22" s="30" customFormat="1" x14ac:dyDescent="0.4">
@@ -2652,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="G30" s="27"/>
       <c r="H30" s="31"/>
@@ -2954,45 +2941,20 @@
       <c r="E39" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F39" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G39" s="20"/>
-      <c r="H39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="L39" s="20"/>
-      <c r="M39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="P39" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
       <c r="Q39" s="27"/>
-      <c r="R39" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="S39" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="T39" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="U39" s="38" t="s">
-        <v>4</v>
-      </c>
+      <c r="R39" s="38"/>
+      <c r="S39" s="38"/>
+      <c r="T39" s="38"/>
+      <c r="U39" s="38"/>
       <c r="V39"/>
     </row>
     <row r="40" spans="1:22" s="30" customFormat="1" x14ac:dyDescent="0.4">
@@ -3011,6 +2973,9 @@
       <c r="E40" s="30" t="b">
         <v>1</v>
       </c>
+      <c r="F40" s="30" t="s">
+        <v>314</v>
+      </c>
       <c r="G40" s="27"/>
       <c r="H40" s="36" t="s">
         <v>290</v>
@@ -3068,20 +3033,45 @@
       <c r="E41" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G41" s="20"/>
+      <c r="H41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="45" t="s">
+        <v>16</v>
+      </c>
       <c r="L41" s="20"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
+      <c r="M41" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="P41" s="45" t="s">
+        <v>16</v>
+      </c>
       <c r="Q41" s="27"/>
-      <c r="R41" s="38"/>
-      <c r="S41" s="38"/>
-      <c r="T41" s="38"/>
-      <c r="U41" s="38"/>
+      <c r="R41" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="S41" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="T41" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="U41" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="V41"/>
     </row>
     <row r="42" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3133,16 +3123,16 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="45" t="b">
+      <c r="D44" s="47" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3165,10 +3155,10 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="17"/>

</xml_diff>

<commit_message>
IHW verbetering foutmelding YAML en correctie jsonschemavariant
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="315">
   <si>
     <t>Name</t>
   </si>
@@ -1114,7 +1114,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1225,6 +1225,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1540,7 +1543,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T41" sqref="T41"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1788,16 +1791,16 @@
       <c r="V6"/>
     </row>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="47" t="b">
+      <c r="D7" s="48" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1817,10 +1820,10 @@
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -2652,10 +2655,18 @@
       <c r="O30" s="32"/>
       <c r="P30" s="32"/>
       <c r="Q30" s="27"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
+      <c r="R30" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="S30" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="T30" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="U30" s="47" t="s">
+        <v>292</v>
+      </c>
       <c r="V30"/>
     </row>
     <row r="31" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3123,16 +3134,16 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="47" t="s">
+      <c r="C44" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="47" t="b">
+      <c r="D44" s="48" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3155,10 +3166,10 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="47"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="17"/>

</xml_diff>

<commit_message>
[ihw] fullrespec nu beschikbaar (yes)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="321">
   <si>
     <t>Name</t>
   </si>
@@ -982,6 +982,12 @@
   </si>
   <si>
     <t>Yes if scalar types may be entered without reference to a UML datatype</t>
+  </si>
+  <si>
+    <t>fullrespec</t>
+  </si>
+  <si>
+    <t>Should a full respec version be generated along with the catalog?</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1132,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1237,6 +1243,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1558,13 +1567,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V134"/>
+  <dimension ref="A1:V135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A72" sqref="A72:XFD72"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1812,16 +1821,16 @@
       <c r="V6"/>
     </row>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="52" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1841,10 +1850,10 @@
       <c r="V7"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="17"/>
@@ -3155,16 +3164,16 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="51" t="s">
+      <c r="C44" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="51" t="b">
+      <c r="D44" s="52" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3187,10 +3196,10 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="51"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
       <c r="G45" s="20"/>
       <c r="L45" s="20"/>
       <c r="M45" s="17"/>
@@ -3515,304 +3524,295 @@
       <c r="U55" s="38"/>
       <c r="V55"/>
     </row>
-    <row r="56" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A56" s="16" t="s">
+    <row r="56" spans="1:22" s="51" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A56" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="B56" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="51" t="s">
+        <v>320</v>
+      </c>
+      <c r="D56" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="Q56" s="27"/>
+    </row>
+    <row r="57" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B57" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C57" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="D56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="16" t="s">
+      <c r="D57" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G56" s="22"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="16"/>
-      <c r="V56"/>
-    </row>
-    <row r="57" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+      <c r="G57" s="22"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="16"/>
+      <c r="V57"/>
+    </row>
+    <row r="58" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="G57" s="27"/>
-      <c r="L57" s="27"/>
-      <c r="Q57" s="27"/>
-    </row>
-    <row r="58" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>311</v>
-      </c>
       <c r="G58" s="27"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
       <c r="L58" s="27"/>
-      <c r="M58" s="34"/>
-      <c r="N58" s="34"/>
-      <c r="O58" s="34"/>
-      <c r="P58" s="34"/>
       <c r="Q58" s="27"/>
     </row>
     <row r="59" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="G59" s="27"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="27"/>
+      <c r="M59" s="34"/>
+      <c r="N59" s="34"/>
+      <c r="O59" s="34"/>
+      <c r="P59" s="34"/>
+      <c r="Q59" s="27"/>
+    </row>
+    <row r="60" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" s="20"/>
-      <c r="L59" s="20"/>
-      <c r="Q59" s="27"/>
-      <c r="V59"/>
-    </row>
-    <row r="60" spans="1:22" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="16" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="Q60" s="27"/>
+      <c r="V60"/>
+    </row>
+    <row r="61" spans="1:22" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B61" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="D60" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="16" t="s">
+      <c r="D61" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="G60" s="22"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="22"/>
-      <c r="R60" s="16"/>
-      <c r="S60" s="16"/>
-      <c r="T60" s="16"/>
-      <c r="U60" s="16"/>
-      <c r="V60"/>
-    </row>
-    <row r="61" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
+      <c r="G61" s="22"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="16"/>
+      <c r="S61" s="16"/>
+      <c r="T61" s="16"/>
+      <c r="U61" s="16"/>
+      <c r="V61"/>
+    </row>
+    <row r="62" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G61" s="20"/>
-      <c r="L61" s="20"/>
-      <c r="Q61" s="27"/>
-      <c r="V61"/>
-    </row>
-    <row r="62" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G62" s="20"/>
       <c r="L62" s="20"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
       <c r="Q62" s="27"/>
-      <c r="R62" s="38"/>
-      <c r="S62" s="38"/>
-      <c r="T62" s="38"/>
-      <c r="U62" s="38"/>
       <c r="V62"/>
     </row>
-    <row r="63" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D63" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>219</v>
+    <row r="63" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="G63" s="20"/>
       <c r="L63" s="20"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
       <c r="Q63" s="27"/>
+      <c r="R63" s="38"/>
+      <c r="S63" s="38"/>
+      <c r="T63" s="38"/>
+      <c r="U63" s="38"/>
       <c r="V63"/>
     </row>
     <row r="64" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>262</v>
-      </c>
-      <c r="B64" t="s">
-        <v>81</v>
-      </c>
-      <c r="C64" t="s">
-        <v>263</v>
-      </c>
-      <c r="D64" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>227</v>
-      </c>
-      <c r="G64" s="27"/>
-      <c r="L64" s="27"/>
+      <c r="A64" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G64" s="20"/>
+      <c r="L64" s="20"/>
       <c r="Q64" s="27"/>
       <c r="V64"/>
     </row>
-    <row r="65" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>262</v>
+      </c>
+      <c r="B65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" t="s">
+        <v>263</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>227</v>
+      </c>
+      <c r="G65" s="27"/>
+      <c r="L65" s="27"/>
+      <c r="Q65" s="27"/>
+      <c r="V65"/>
+    </row>
+    <row r="66" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
+      <c r="D66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="G65" s="20"/>
-      <c r="L65" s="20"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="17"/>
-      <c r="Q65" s="27"/>
-      <c r="R65" s="38"/>
-      <c r="S65" s="38"/>
-      <c r="T65" s="38"/>
-      <c r="U65" s="38"/>
-      <c r="V65"/>
-    </row>
-    <row r="66" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="G66" s="20"/>
       <c r="L66" s="20"/>
@@ -3827,24 +3827,24 @@
       <c r="U66" s="38"/>
       <c r="V66"/>
     </row>
-    <row r="67" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>208</v>
+        <v>297</v>
       </c>
       <c r="G67" s="20"/>
       <c r="L67" s="20"/>
@@ -3859,27 +3859,31 @@
       <c r="U67" s="38"/>
       <c r="V67"/>
     </row>
-    <row r="68" spans="1:22" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="D68" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>255</v>
+    <row r="68" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="G68" s="20"/>
       <c r="L68" s="20"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
+      <c r="O68" s="17"/>
+      <c r="P68" s="17"/>
       <c r="Q68" s="27"/>
       <c r="R68" s="38"/>
       <c r="S68" s="38"/>
@@ -3887,190 +3891,186 @@
       <c r="U68" s="38"/>
       <c r="V68"/>
     </row>
-    <row r="69" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:22" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D69" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="G69" s="20"/>
+      <c r="L69" s="20"/>
+      <c r="Q69" s="27"/>
+      <c r="R69" s="38"/>
+      <c r="S69" s="38"/>
+      <c r="T69" s="38"/>
+      <c r="U69" s="38"/>
+      <c r="V69"/>
+    </row>
+    <row r="70" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D69" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G69" s="20"/>
-      <c r="H69" s="2" t="s">
+      <c r="D70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" s="20"/>
+      <c r="H70" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I69" s="38" t="s">
+      <c r="I70" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="J69" s="38" t="s">
+      <c r="J70" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="K69" s="38" t="s">
+      <c r="K70" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="L69" s="20"/>
-      <c r="M69" s="33" t="s">
+      <c r="L70" s="20"/>
+      <c r="M70" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="N69" s="38" t="s">
+      <c r="N70" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="O69" s="38" t="s">
+      <c r="O70" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="P69" s="38" t="s">
+      <c r="P70" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="38" t="s">
+      <c r="Q70" s="27"/>
+      <c r="R70" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="S69" s="38" t="s">
+      <c r="S70" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="T69" s="38" t="s">
+      <c r="T70" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="U69" s="38" t="s">
+      <c r="U70" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="V69"/>
-    </row>
-    <row r="70" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="48" t="s">
+      <c r="V70"/>
+    </row>
+    <row r="71" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="B70" s="48" t="s">
+      <c r="B71" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="48" t="s">
+      <c r="C71" s="48" t="s">
         <v>314</v>
       </c>
-      <c r="D70" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="48"/>
-      <c r="G70" s="20"/>
-      <c r="L70" s="20"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="27"/>
-      <c r="R70" s="38"/>
-      <c r="S70" s="38"/>
-      <c r="T70" s="38"/>
-      <c r="U70" s="38"/>
-      <c r="V70"/>
-    </row>
-    <row r="71" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D71" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="D71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="48"/>
       <c r="G71" s="20"/>
       <c r="L71" s="20"/>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
       <c r="Q71" s="27"/>
+      <c r="R71" s="38"/>
+      <c r="S71" s="38"/>
+      <c r="T71" s="38"/>
+      <c r="U71" s="38"/>
       <c r="V71"/>
     </row>
-    <row r="72" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="40" t="s">
+    <row r="72" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="20"/>
+      <c r="L72" s="20"/>
+      <c r="Q72" s="27"/>
+      <c r="V72"/>
+    </row>
+    <row r="73" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="40" t="s">
         <v>317</v>
       </c>
-      <c r="B72" s="40" t="s">
+      <c r="B73" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="40" t="s">
+      <c r="C73" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="D72" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="G72" s="27"/>
-      <c r="L72" s="27"/>
-      <c r="Q72" s="27"/>
-    </row>
-    <row r="73" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="20"/>
-      <c r="L73" s="20"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
+      <c r="D73" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="27"/>
+      <c r="L73" s="27"/>
       <c r="Q73" s="27"/>
-      <c r="R73" s="38"/>
-      <c r="S73" s="38"/>
-      <c r="T73" s="38"/>
-      <c r="U73" s="38"/>
-      <c r="V73"/>
     </row>
     <row r="74" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>76</v>
+        <v>218</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>77</v>
+        <v>230</v>
       </c>
       <c r="D74" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G74" s="20"/>
       <c r="L74" s="20"/>
@@ -4085,451 +4085,455 @@
       <c r="U74" s="38"/>
       <c r="V74"/>
     </row>
-    <row r="75" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="20"/>
+      <c r="L75" s="20"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="27"/>
+      <c r="R75" s="38"/>
+      <c r="S75" s="38"/>
+      <c r="T75" s="38"/>
+      <c r="U75" s="38"/>
+      <c r="V75"/>
+    </row>
+    <row r="76" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="33"/>
-      <c r="G75" s="20"/>
-      <c r="H75" s="38" t="s">
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="33"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="I75" s="38" t="s">
+      <c r="I76" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="J75" s="38" t="s">
+      <c r="J76" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="K75" s="38" t="s">
+      <c r="K76" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="L75" s="27"/>
-      <c r="M75" s="38" t="s">
+      <c r="L76" s="27"/>
+      <c r="M76" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="N75" s="38" t="s">
+      <c r="N76" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="O75" s="38" t="s">
+      <c r="O76" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="P75" s="38" t="s">
+      <c r="P76" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="Q75" s="27"/>
-      <c r="R75" s="38" t="s">
+      <c r="Q76" s="27"/>
+      <c r="R76" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="S75" s="38" t="s">
+      <c r="S76" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="T75" s="38" t="s">
+      <c r="T76" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="U75" s="38" t="s">
+      <c r="U76" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="V75"/>
-    </row>
-    <row r="76" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
+      <c r="V76"/>
+    </row>
+    <row r="77" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="G76" s="20"/>
-      <c r="L76" s="20"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="27"/>
-      <c r="R76" s="38"/>
-      <c r="S76" s="38"/>
-      <c r="T76" s="38"/>
-      <c r="U76" s="38"/>
-      <c r="V76"/>
-    </row>
-    <row r="77" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>285</v>
       </c>
       <c r="G77" s="20"/>
       <c r="L77" s="20"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="27"/>
+      <c r="R77" s="38"/>
+      <c r="S77" s="38"/>
+      <c r="T77" s="38"/>
+      <c r="U77" s="38"/>
       <c r="V77"/>
     </row>
-    <row r="78" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>19</v>
+    <row r="78" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>285</v>
       </c>
       <c r="G78" s="20"/>
       <c r="L78" s="20"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
       <c r="Q78" s="27"/>
-      <c r="R78" s="38"/>
-      <c r="S78" s="38"/>
-      <c r="T78" s="38"/>
-      <c r="U78" s="38"/>
       <c r="V78"/>
     </row>
-    <row r="79" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>211</v>
+    <row r="79" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G79" s="20"/>
       <c r="L79" s="20"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
       <c r="Q79" s="27"/>
+      <c r="R79" s="38"/>
+      <c r="S79" s="38"/>
+      <c r="T79" s="38"/>
+      <c r="U79" s="38"/>
       <c r="V79"/>
     </row>
-    <row r="80" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
+    <row r="80" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="G80" s="20"/>
-      <c r="H80" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>292</v>
-      </c>
       <c r="L80" s="20"/>
-      <c r="M80" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="N80" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="P80" s="17" t="s">
-        <v>293</v>
-      </c>
       <c r="Q80" s="27"/>
-      <c r="R80" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="S80" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="T80" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="U80" s="38" t="s">
-        <v>294</v>
-      </c>
       <c r="V80"/>
     </row>
     <row r="81" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" s="20"/>
+      <c r="H81" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="J81" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="K81" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="L81" s="20"/>
+      <c r="M81" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="N81" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="O81" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="P81" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q81" s="27"/>
+      <c r="R81" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="S81" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="T81" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="U81" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="V81"/>
+    </row>
+    <row r="82" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G81" s="20"/>
-      <c r="L81" s="20"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="27"/>
-      <c r="R81" s="38"/>
-      <c r="S81" s="38"/>
-      <c r="T81" s="38"/>
-      <c r="U81" s="38"/>
-      <c r="V81"/>
-    </row>
-    <row r="82" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="G82" s="20"/>
       <c r="L82" s="20"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
       <c r="Q82" s="27"/>
+      <c r="R82" s="38"/>
+      <c r="S82" s="38"/>
+      <c r="T82" s="38"/>
+      <c r="U82" s="38"/>
       <c r="V82"/>
     </row>
     <row r="83" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D83" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="G83" s="20"/>
       <c r="L83" s="20"/>
       <c r="Q83" s="27"/>
       <c r="V83"/>
     </row>
-    <row r="84" spans="1:22" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>96</v>
+    <row r="84" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G84" s="20"/>
       <c r="L84" s="20"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
       <c r="Q84" s="27"/>
-      <c r="R84" s="38"/>
-      <c r="S84" s="38"/>
-      <c r="T84" s="38"/>
-      <c r="U84" s="38"/>
       <c r="V84"/>
     </row>
-    <row r="85" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:22" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D85" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E85" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G85" s="20"/>
-      <c r="H85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L85" s="20"/>
-      <c r="M85" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N85" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O85" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P85" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="27"/>
-      <c r="R85" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="S85" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="T85" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="U85" s="38" t="s">
-        <v>4</v>
-      </c>
+      <c r="R85" s="38"/>
+      <c r="S85" s="38"/>
+      <c r="T85" s="38"/>
+      <c r="U85" s="38"/>
       <c r="V85"/>
     </row>
     <row r="86" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="20"/>
+      <c r="H86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L86" s="20"/>
+      <c r="M86" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O86" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P86" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q86" s="27"/>
+      <c r="R86" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="S86" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="T86" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="U86" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="V86"/>
+    </row>
+    <row r="87" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G86" s="20"/>
-      <c r="L86" s="20"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="27"/>
-      <c r="R86" s="38"/>
-      <c r="S86" s="38"/>
-      <c r="T86" s="38"/>
-      <c r="U86" s="38"/>
-      <c r="V86"/>
-    </row>
-    <row r="87" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D87" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="G87" s="27"/>
-      <c r="L87" s="27"/>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="20"/>
+      <c r="L87" s="20"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="27"/>
       <c r="R87" s="38"/>
       <c r="S87" s="38"/>
@@ -4537,31 +4541,27 @@
       <c r="U87" s="38"/>
       <c r="V87"/>
     </row>
-    <row r="88" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="G88" s="20"/>
-      <c r="L88" s="20"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
+    <row r="88" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B88" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="G88" s="27"/>
+      <c r="L88" s="27"/>
       <c r="Q88" s="27"/>
       <c r="R88" s="38"/>
       <c r="S88" s="38"/>
@@ -4569,24 +4569,24 @@
       <c r="U88" s="38"/>
       <c r="V88"/>
     </row>
-    <row r="89" spans="1:22" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="D89" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>251</v>
+    <row r="89" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="12" t="s">
+        <v>252</v>
       </c>
       <c r="G89" s="20"/>
       <c r="L89" s="20"/>
@@ -4601,30 +4601,31 @@
       <c r="U89" s="38"/>
       <c r="V89"/>
     </row>
-    <row r="90" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>285</v>
+    <row r="90" spans="1:22" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="D90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="G90" s="20"/>
-      <c r="I90" s="35"/>
-      <c r="J90" s="35"/>
-      <c r="K90" s="35"/>
       <c r="L90" s="20"/>
-      <c r="M90" s="35"/>
-      <c r="N90" s="35"/>
-      <c r="O90" s="35"/>
-      <c r="P90" s="35"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
       <c r="Q90" s="27"/>
       <c r="R90" s="38"/>
       <c r="S90" s="38"/>
@@ -4632,31 +4633,30 @@
       <c r="U90" s="38"/>
       <c r="V90"/>
     </row>
-    <row r="91" spans="1:22" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F91" s="2" t="s">
-        <v>16</v>
+      <c r="F91" s="17" t="s">
+        <v>285</v>
       </c>
       <c r="G91" s="20"/>
+      <c r="I91" s="35"/>
+      <c r="J91" s="35"/>
+      <c r="K91" s="35"/>
       <c r="L91" s="20"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
+      <c r="M91" s="35"/>
+      <c r="N91" s="35"/>
+      <c r="O91" s="35"/>
+      <c r="P91" s="35"/>
       <c r="Q91" s="27"/>
       <c r="R91" s="38"/>
       <c r="S91" s="38"/>
@@ -4664,70 +4664,70 @@
       <c r="U91" s="38"/>
       <c r="V91"/>
     </row>
-    <row r="92" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
+    <row r="92" spans="1:22" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="20"/>
+      <c r="L92" s="20"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
+      <c r="Q92" s="27"/>
+      <c r="R92" s="38"/>
+      <c r="S92" s="38"/>
+      <c r="T92" s="38"/>
+      <c r="U92" s="38"/>
+      <c r="V92"/>
+    </row>
+    <row r="93" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
         <v>300</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>10</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>301</v>
       </c>
-      <c r="D92" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="D93" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
         <v>285</v>
       </c>
-      <c r="G92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="Q92" s="27"/>
-    </row>
-    <row r="93" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="G93" s="20"/>
-      <c r="L93" s="20"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="17"/>
+      <c r="G93" s="27"/>
+      <c r="L93" s="27"/>
       <c r="Q93" s="27"/>
-      <c r="R93" s="38"/>
-      <c r="S93" s="38"/>
-      <c r="T93" s="38"/>
-      <c r="U93" s="38"/>
-      <c r="V93"/>
     </row>
     <row r="94" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D94" s="2" t="b">
         <v>0</v>
@@ -4735,8 +4735,8 @@
       <c r="E94" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F94" s="2" t="s">
-        <v>16</v>
+      <c r="F94" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="G94" s="20"/>
       <c r="L94" s="20"/>
@@ -4751,21 +4751,24 @@
       <c r="U94" s="38"/>
       <c r="V94"/>
     </row>
-    <row r="95" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G95" s="20"/>
       <c r="L95" s="20"/>
@@ -4782,22 +4785,19 @@
     </row>
     <row r="96" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="G96" s="20"/>
       <c r="L96" s="20"/>
@@ -4812,96 +4812,104 @@
       <c r="U96" s="38"/>
       <c r="V96"/>
     </row>
-    <row r="97" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G97" s="20"/>
+      <c r="L97" s="20"/>
+      <c r="M97" s="17"/>
+      <c r="N97" s="17"/>
+      <c r="O97" s="17"/>
+      <c r="P97" s="17"/>
+      <c r="Q97" s="27"/>
+      <c r="R97" s="38"/>
+      <c r="S97" s="38"/>
+      <c r="T97" s="38"/>
+      <c r="U97" s="38"/>
+      <c r="V97"/>
+    </row>
+    <row r="98" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97" s="20"/>
-      <c r="H97" s="38" t="s">
+      <c r="D98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" s="20"/>
+      <c r="H98" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="I97" s="38" t="s">
+      <c r="I98" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="J97" s="38" t="s">
+      <c r="J98" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="K97" s="38" t="s">
+      <c r="K98" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="L97" s="27"/>
-      <c r="M97" s="38" t="s">
+      <c r="L98" s="27"/>
+      <c r="M98" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="N97" s="38" t="s">
+      <c r="N98" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="O97" s="38" t="s">
+      <c r="O98" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="P97" s="38" t="s">
+      <c r="P98" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="Q97" s="27"/>
-      <c r="R97" s="38" t="s">
+      <c r="Q98" s="27"/>
+      <c r="R98" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="S97" s="38" t="s">
+      <c r="S98" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="T97" s="38" t="s">
+      <c r="T98" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="U97" s="38" t="s">
+      <c r="U98" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="V97"/>
-    </row>
-    <row r="98" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="G98" s="20"/>
-      <c r="L98" s="20"/>
-      <c r="Q98" s="27"/>
       <c r="V98"/>
     </row>
     <row r="99" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D99" s="7" t="b">
         <v>1</v>
@@ -4919,97 +4927,64 @@
     </row>
     <row r="100" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D100" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E100" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>16</v>
+        <v>219</v>
       </c>
       <c r="G100" s="20"/>
       <c r="L100" s="20"/>
       <c r="Q100" s="27"/>
       <c r="V100"/>
     </row>
-    <row r="101" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B101" s="2" t="s">
+    <row r="101" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B101" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
+      <c r="C101" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G101" s="20"/>
-      <c r="H101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L101" s="20"/>
-      <c r="M101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P101" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="Q101" s="27"/>
-      <c r="R101" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="S101" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="T101" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="U101" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="V101"/>
     </row>
     <row r="102" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
         <v>1</v>
@@ -5057,23 +5032,23 @@
     </row>
     <row r="103" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D103" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G103" s="20"/>
       <c r="H103" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>4</v>
@@ -5086,7 +5061,7 @@
       </c>
       <c r="L103" s="20"/>
       <c r="M103" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N103" s="17" t="s">
         <v>4</v>
@@ -5099,7 +5074,7 @@
       </c>
       <c r="Q103" s="27"/>
       <c r="R103" s="38" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="S103" s="38" t="s">
         <v>4</v>
@@ -5112,165 +5087,166 @@
       </c>
       <c r="V103"/>
     </row>
-    <row r="104" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" s="20"/>
+      <c r="H104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L104" s="20"/>
+      <c r="M104" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q104" s="27"/>
+      <c r="R104" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="S104" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="T104" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="U104" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="V104"/>
+    </row>
+    <row r="105" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G104" s="20"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="L104" s="20"/>
-      <c r="M104" s="17"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="27"/>
-      <c r="R104" s="38"/>
-      <c r="S104" s="38"/>
-      <c r="T104" s="38"/>
-      <c r="U104" s="38"/>
-      <c r="V104"/>
-    </row>
-    <row r="105" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>302</v>
-      </c>
-      <c r="B105" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" t="s">
-        <v>303</v>
-      </c>
-      <c r="D105" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" t="s">
-        <v>4</v>
-      </c>
-      <c r="G105" s="27"/>
+      <c r="D105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" s="20"/>
       <c r="H105"/>
       <c r="I105"/>
       <c r="J105"/>
       <c r="K105"/>
-      <c r="L105" s="27"/>
-      <c r="M105"/>
-      <c r="N105"/>
-      <c r="O105"/>
-      <c r="P105"/>
+      <c r="L105" s="20"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="17"/>
+      <c r="O105" s="17"/>
+      <c r="P105" s="17"/>
       <c r="Q105" s="27"/>
-      <c r="R105"/>
-      <c r="S105"/>
-      <c r="T105"/>
-      <c r="U105"/>
-    </row>
-    <row r="106" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A106" s="7" t="s">
+      <c r="R105" s="38"/>
+      <c r="S105" s="38"/>
+      <c r="T105" s="38"/>
+      <c r="U105" s="38"/>
+      <c r="V105"/>
+    </row>
+    <row r="106" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>302</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>303</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="27"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="L106" s="27"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+      <c r="P106"/>
+      <c r="Q106" s="27"/>
+      <c r="R106"/>
+      <c r="S106"/>
+      <c r="T106"/>
+      <c r="U106"/>
+    </row>
+    <row r="107" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B107" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" s="20"/>
-      <c r="L106" s="20"/>
-      <c r="Q106" s="27"/>
-    </row>
-    <row r="107" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
+      <c r="D107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G107" s="20"/>
-      <c r="H107" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L107" s="20"/>
-      <c r="M107" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="Q107" s="27"/>
-      <c r="R107" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="S107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="T107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="U107" s="38" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="108" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>239</v>
+        <v>127</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>1</v>
@@ -5320,200 +5296,253 @@
     </row>
     <row r="109" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="20"/>
+      <c r="H109" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="20"/>
+      <c r="M109" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="27"/>
+      <c r="R109" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="S109" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="T109" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="U109" s="38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F109" s="2" t="s">
+      <c r="D110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G109" s="20"/>
-      <c r="L109" s="20"/>
-      <c r="M109" s="17"/>
-      <c r="N109" s="17"/>
-      <c r="O109" s="17"/>
-      <c r="P109" s="17"/>
-      <c r="Q109" s="27"/>
-      <c r="R109" s="38"/>
-      <c r="S109" s="38"/>
-      <c r="T109" s="38"/>
-      <c r="U109" s="38"/>
-    </row>
-    <row r="110" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="49" t="s">
+      <c r="G110" s="20"/>
+      <c r="L110" s="20"/>
+      <c r="M110" s="17"/>
+      <c r="N110" s="17"/>
+      <c r="O110" s="17"/>
+      <c r="P110" s="17"/>
+      <c r="Q110" s="27"/>
+      <c r="R110" s="38"/>
+      <c r="S110" s="38"/>
+      <c r="T110" s="38"/>
+      <c r="U110" s="38"/>
+    </row>
+    <row r="111" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="49" t="s">
         <v>315</v>
       </c>
-      <c r="B110" s="49" t="s">
+      <c r="B111" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C110" s="49" t="s">
+      <c r="C111" s="49" t="s">
         <v>316</v>
       </c>
-      <c r="D110" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="G110" s="27"/>
-      <c r="H110" s="49" t="s">
+      <c r="D111" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="27"/>
+      <c r="H111" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="I110" s="49" t="s">
+      <c r="I111" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="J110" s="49" t="s">
+      <c r="J111" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="K110" s="49" t="s">
+      <c r="K111" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="L110" s="27"/>
-      <c r="M110" s="49" t="s">
+      <c r="L111" s="27"/>
+      <c r="M111" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="N110" s="49" t="s">
+      <c r="N111" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="O110" s="49" t="s">
+      <c r="O111" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="P110" s="49" t="s">
+      <c r="P111" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="Q110" s="27"/>
-      <c r="R110" s="49" t="s">
+      <c r="Q111" s="27"/>
+      <c r="R111" s="49" t="s">
         <v>291</v>
       </c>
-      <c r="S110" s="49" t="s">
+      <c r="S111" s="49" t="s">
         <v>291</v>
       </c>
-      <c r="T110" s="49" t="s">
+      <c r="T111" s="49" t="s">
         <v>291</v>
       </c>
-      <c r="U110" s="49" t="s">
+      <c r="U111" s="49" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="111" spans="1:22" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A111" s="26" t="s">
+    <row r="112" spans="1:22" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A112" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B112" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C111" s="26" t="s">
+      <c r="C112" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="D111" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="26" t="s">
+      <c r="D112" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="G111" s="27"/>
-      <c r="H111" s="26"/>
-      <c r="I111" s="26"/>
-      <c r="J111" s="26"/>
-      <c r="K111" s="26"/>
-      <c r="L111" s="27"/>
-      <c r="M111" s="26"/>
-      <c r="Q111" s="27"/>
-      <c r="R111" s="38"/>
-      <c r="S111" s="38"/>
-      <c r="T111" s="38"/>
-      <c r="U111" s="38"/>
-    </row>
-    <row r="112" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G112" s="20"/>
-      <c r="L112" s="20"/>
-      <c r="M112" s="17"/>
-      <c r="N112" s="17"/>
-      <c r="O112" s="17"/>
-      <c r="P112" s="17"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="26"/>
+      <c r="I112" s="26"/>
+      <c r="J112" s="26"/>
+      <c r="K112" s="26"/>
+      <c r="L112" s="27"/>
+      <c r="M112" s="26"/>
       <c r="Q112" s="27"/>
       <c r="R112" s="38"/>
       <c r="S112" s="38"/>
       <c r="T112" s="38"/>
       <c r="U112" s="38"/>
     </row>
-    <row r="113" spans="22:22" x14ac:dyDescent="0.4">
-      <c r="V113"/>
-    </row>
-    <row r="114" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G113" s="20"/>
+      <c r="L113" s="20"/>
+      <c r="M113" s="17"/>
+      <c r="N113" s="17"/>
+      <c r="O113" s="17"/>
+      <c r="P113" s="17"/>
+      <c r="Q113" s="27"/>
+      <c r="R113" s="38"/>
+      <c r="S113" s="38"/>
+      <c r="T113" s="38"/>
+      <c r="U113" s="38"/>
+    </row>
+    <row r="114" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V114"/>
     </row>
-    <row r="115" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V115"/>
     </row>
-    <row r="116" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V116"/>
     </row>
-    <row r="117" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V117"/>
     </row>
-    <row r="118" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V118"/>
     </row>
-    <row r="119" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V119"/>
     </row>
-    <row r="120" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V120"/>
     </row>
-    <row r="121" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V121"/>
     </row>
-    <row r="122" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V122"/>
     </row>
-    <row r="123" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V123"/>
     </row>
-    <row r="124" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V124"/>
     </row>
-    <row r="125" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V125"/>
     </row>
-    <row r="126" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V126"/>
     </row>
-    <row r="127" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V127"/>
     </row>
-    <row r="128" spans="22:22" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V128"/>
     </row>
     <row r="129" spans="22:22" x14ac:dyDescent="0.4">
@@ -5533,6 +5562,9 @@
     </row>
     <row r="134" spans="22:22" x14ac:dyDescent="0.4">
       <c r="V134"/>
+    </row>
+    <row r="135" spans="22:22" x14ac:dyDescent="0.4">
+      <c r="V135"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5548,7 +5580,7 @@
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F58" r:id="rId3"/>
+    <hyperlink ref="F59" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
IHW: Instellen property officename op de juiste waarde.
De bestandsnamen moeten worden opgebouwd als:

officename = [model-abbreviation]-cat

voor het genereren van een GIT bestand:

./data/SIM-IMWA-Afvalwaterketen.html

Bugfix.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\IHW\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FDD36B-8471-479F-9B1A-39657498FDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48B8EFA-5D42-4259-96C9-B067BD272EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,9 +838,6 @@
     <t>click</t>
   </si>
   <si>
-    <t>[project-name]-[application-name]-[phase]-[release]</t>
-  </si>
-  <si>
     <t>createofficevariant</t>
   </si>
   <si>
@@ -1007,6 +1004,9 @@
   </si>
   <si>
     <t>/Aquo-standaard/[model-abbreviation]</t>
+  </si>
+  <si>
+    <t>[model-abbreviation]-cat</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1507,10 @@
   <dimension ref="A1:Y136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F61" sqref="F61"/>
+      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1616,51 +1616,51 @@
       <c r="F2" s="3"/>
       <c r="G2" s="14"/>
       <c r="H2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>296</v>
-      </c>
       <c r="J2" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="S2" s="14"/>
       <c r="T2" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="X2" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Y2" s="23"/>
     </row>
@@ -2053,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G18" s="15"/>
       <c r="M18" s="15"/>
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G20" s="15"/>
       <c r="M20" s="15"/>
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G21" s="15"/>
       <c r="M21" s="15"/>
@@ -2545,25 +2545,25 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G30" s="15"/>
       <c r="M30" s="15"/>
       <c r="S30" s="15"/>
       <c r="T30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y30" s="24"/>
     </row>
@@ -2683,22 +2683,22 @@
     </row>
     <row r="34" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="G34" s="15"/>
       <c r="M34" s="15"/>
@@ -2731,13 +2731,13 @@
     </row>
     <row r="36" spans="1:25" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D36" s="20" t="b">
         <v>0</v>
@@ -2842,55 +2842,55 @@
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M40" s="15"/>
       <c r="N40" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S40" s="15"/>
       <c r="T40" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y40" s="24"/>
     </row>
@@ -3122,51 +3122,51 @@
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M49" s="16"/>
       <c r="N49" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S49" s="16"/>
       <c r="T49" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V49" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y49" s="24"/>
     </row>
@@ -3316,13 +3316,13 @@
     </row>
     <row r="56" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
@@ -3340,13 +3340,13 @@
     </row>
     <row r="57" spans="1:25" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D57" s="12" t="b">
         <v>0</v>
@@ -3355,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="12"/>
@@ -3375,22 +3375,22 @@
     </row>
     <row r="58" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="C58" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="D58" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="D58" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>309</v>
       </c>
       <c r="G58" s="15"/>
       <c r="M58" s="15"/>
@@ -3399,13 +3399,13 @@
     </row>
     <row r="59" spans="1:25" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>89</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D59" s="6" t="b">
         <v>0</v>
@@ -3414,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="19"/>
@@ -3448,7 +3448,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G60" s="15"/>
       <c r="M60" s="15"/>
@@ -3631,7 +3631,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G67" s="15"/>
       <c r="M67" s="15"/>
@@ -3704,51 +3704,51 @@
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M70" s="15"/>
       <c r="N70" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S70" s="15"/>
       <c r="T70" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U70" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V70" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X70" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y70" s="24"/>
     </row>
@@ -3760,7 +3760,7 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D71" s="2" t="b">
         <v>0</v>
@@ -3799,13 +3799,13 @@
     </row>
     <row r="73" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
@@ -3887,51 +3887,51 @@
       </c>
       <c r="G76" s="15"/>
       <c r="H76" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q76" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R76" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S76" s="15"/>
       <c r="T76" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U76" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V76" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W76" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X76" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y76" s="24"/>
     </row>
@@ -3952,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
       <c r="G77" s="15"/>
       <c r="M77" s="15"/>
@@ -3976,7 +3976,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G78" s="15"/>
       <c r="M78" s="15"/>
@@ -4049,51 +4049,51 @@
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M81" s="15"/>
       <c r="N81" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q81" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="R81" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="S81" s="15"/>
       <c r="T81" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="U81" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V81" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W81" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="X81" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Y81" s="24"/>
     </row>
@@ -4171,13 +4171,13 @@
     </row>
     <row r="85" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B85" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D85" s="20" t="b">
         <v>0</v>
@@ -4409,7 +4409,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G92" s="15"/>
       <c r="M92" s="15"/>
@@ -4442,13 +4442,13 @@
     </row>
     <row r="94" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -4457,7 +4457,7 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G94" s="15"/>
       <c r="M94" s="15"/>
@@ -4575,51 +4575,51 @@
       </c>
       <c r="G99" s="15"/>
       <c r="H99" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M99" s="15"/>
       <c r="N99" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P99" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q99" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R99" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S99" s="15"/>
       <c r="T99" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U99" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V99" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W99" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X99" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y99" s="24"/>
     </row>
@@ -4924,13 +4924,13 @@
     </row>
     <row r="107" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B107" t="s">
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D107" t="b">
         <v>0</v>
@@ -5134,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G111" s="15"/>
       <c r="M111" s="15"/>
@@ -5143,13 +5143,13 @@
     </row>
     <row r="112" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D112" s="2" t="b">
         <v>1</v>
@@ -5159,51 +5159,51 @@
       </c>
       <c r="G112" s="15"/>
       <c r="H112" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M112" s="15"/>
       <c r="N112" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O112" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P112" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q112" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R112" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S112" s="15"/>
       <c r="T112" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U112" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V112" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W112" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X112" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y112" s="1"/>
     </row>

</xml_diff>

<commit_message>
IHW: Introductie van logisch model.
Dit is doorgevoerd in
- Properties file (xlsx), unu gebaseerd op UGM settings
- Metamodel en tagged value set
- notesrules
- visuals voor Toolbox.

De details moeten nog verder worden uitgewerkt, in overleg met IHW.

Zie #499

Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\IHW\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48B8EFA-5D42-4259-96C9-B067BD272EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1173ECB6-CF38-404E-A08B-5BF5094C15DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHW" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="334">
   <si>
     <t>Name</t>
   </si>
@@ -1007,6 +1007,27 @@
   </si>
   <si>
     <t>[model-abbreviation]-cat</t>
+  </si>
+  <si>
+    <t>LM: minimum</t>
+  </si>
+  <si>
+    <t>LM: uitgebreid</t>
+  </si>
+  <si>
+    <t>LM: opleveren</t>
+  </si>
+  <si>
+    <t>LM: docrelease</t>
+  </si>
+  <si>
+    <t>LM: regtest</t>
+  </si>
+  <si>
+    <t>IHWLM</t>
+  </si>
+  <si>
+    <t>LM</t>
   </si>
 </sst>
 </file>
@@ -1504,13 +1525,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y136"/>
+  <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
+      <selection pane="bottomRight" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1538,10 +1559,16 @@
     <col min="22" max="22" width="15.69140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.765625" customWidth="1"/>
     <col min="24" max="24" width="11.921875" customWidth="1"/>
-    <col min="25" max="25" width="27.3046875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="5.4609375" style="18" customWidth="1"/>
+    <col min="26" max="26" width="12.61328125" customWidth="1"/>
+    <col min="27" max="27" width="16.07421875" customWidth="1"/>
+    <col min="28" max="28" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.765625" customWidth="1"/>
+    <col min="30" max="30" width="11.921875" customWidth="1"/>
+    <col min="31" max="31" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1608,11 +1635,27 @@
       <c r="X1" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="Y1" s="22" t="s">
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AE1" s="22" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:31" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="14"/>
       <c r="H2" s="3" t="s">
@@ -1662,9 +1705,25 @@
       <c r="X2" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="Y2" s="23"/>
-    </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="AE2" s="23"/>
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -1683,9 +1742,10 @@
       <c r="G3" s="15"/>
       <c r="M3" s="15"/>
       <c r="S3" s="15"/>
-      <c r="Y3" s="24"/>
-    </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y3" s="15"/>
+      <c r="AE3" s="24"/>
+    </row>
+    <row r="4" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1707,9 +1767,10 @@
       <c r="G4" s="15"/>
       <c r="M4" s="15"/>
       <c r="S4" s="15"/>
-      <c r="Y4" s="24"/>
-    </row>
-    <row r="5" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y4" s="15"/>
+      <c r="AE4" s="24"/>
+    </row>
+    <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1731,9 +1792,10 @@
       <c r="G5" s="15"/>
       <c r="M5" s="15"/>
       <c r="S5" s="15"/>
-      <c r="Y5" s="24"/>
-    </row>
-    <row r="6" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y5" s="15"/>
+      <c r="AE5" s="24"/>
+    </row>
+    <row r="6" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>157</v>
       </c>
@@ -1752,9 +1814,10 @@
       <c r="G6" s="15"/>
       <c r="M6" s="15"/>
       <c r="S6" s="15"/>
-      <c r="Y6" s="24"/>
-    </row>
-    <row r="7" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y6" s="15"/>
+      <c r="AE6" s="24"/>
+    </row>
+    <row r="7" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -1773,9 +1836,10 @@
       <c r="G7" s="15"/>
       <c r="M7" s="15"/>
       <c r="S7" s="15"/>
-      <c r="Y7" s="24"/>
-    </row>
-    <row r="8" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y7" s="15"/>
+      <c r="AE7" s="24"/>
+    </row>
+    <row r="8" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -1783,9 +1847,10 @@
       <c r="G8" s="15"/>
       <c r="M8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="Y8" s="24"/>
-    </row>
-    <row r="9" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y8" s="15"/>
+      <c r="AE8" s="24"/>
+    </row>
+    <row r="9" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>160</v>
       </c>
@@ -1807,9 +1872,10 @@
       <c r="G9" s="15"/>
       <c r="M9" s="15"/>
       <c r="S9" s="15"/>
-      <c r="Y9" s="24"/>
-    </row>
-    <row r="10" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y9" s="15"/>
+      <c r="AE9" s="24"/>
+    </row>
+    <row r="10" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1831,9 +1897,10 @@
       <c r="G10" s="15"/>
       <c r="M10" s="15"/>
       <c r="S10" s="15"/>
-      <c r="Y10" s="24"/>
-    </row>
-    <row r="11" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y10" s="15"/>
+      <c r="AE10" s="24"/>
+    </row>
+    <row r="11" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>162</v>
       </c>
@@ -1852,9 +1919,10 @@
       <c r="G11" s="15"/>
       <c r="M11" s="15"/>
       <c r="S11" s="15"/>
-      <c r="Y11" s="24"/>
-    </row>
-    <row r="12" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y11" s="15"/>
+      <c r="AE11" s="24"/>
+    </row>
+    <row r="12" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>135</v>
       </c>
@@ -1876,9 +1944,10 @@
       <c r="G12" s="15"/>
       <c r="M12" s="15"/>
       <c r="S12" s="15"/>
-      <c r="Y12" s="24"/>
-    </row>
-    <row r="13" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y12" s="15"/>
+      <c r="AE12" s="24"/>
+    </row>
+    <row r="13" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>244</v>
       </c>
@@ -1900,9 +1969,10 @@
       <c r="G13" s="15"/>
       <c r="M13" s="15"/>
       <c r="S13" s="15"/>
-      <c r="Y13" s="24"/>
-    </row>
-    <row r="14" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y13" s="15"/>
+      <c r="AE13" s="24"/>
+    </row>
+    <row r="14" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1924,9 +1994,10 @@
       <c r="G14" s="15"/>
       <c r="M14" s="15"/>
       <c r="S14" s="15"/>
-      <c r="Y14" s="24"/>
-    </row>
-    <row r="15" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y14" s="15"/>
+      <c r="AE14" s="24"/>
+    </row>
+    <row r="15" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1990,9 +2061,25 @@
       <c r="X15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Y15" s="24"/>
-    </row>
-    <row r="16" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE15" s="24"/>
+    </row>
+    <row r="16" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2014,9 +2101,10 @@
       <c r="G16" s="15"/>
       <c r="M16" s="15"/>
       <c r="S16" s="15"/>
-      <c r="Y16" s="24"/>
-    </row>
-    <row r="17" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y16" s="15"/>
+      <c r="AE16" s="24"/>
+    </row>
+    <row r="17" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>222</v>
       </c>
@@ -2038,9 +2126,10 @@
       <c r="G17" s="15"/>
       <c r="M17" s="15"/>
       <c r="S17" s="15"/>
-      <c r="Y17" s="24"/>
-    </row>
-    <row r="18" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y17" s="15"/>
+      <c r="AE17" s="24"/>
+    </row>
+    <row r="18" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>224</v>
       </c>
@@ -2058,9 +2147,10 @@
       <c r="G18" s="15"/>
       <c r="M18" s="15"/>
       <c r="S18" s="15"/>
-      <c r="Y18" s="24"/>
-    </row>
-    <row r="19" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y18" s="15"/>
+      <c r="AE18" s="24"/>
+    </row>
+    <row r="19" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -2079,9 +2169,10 @@
       <c r="G19" s="15"/>
       <c r="M19" s="15"/>
       <c r="S19" s="15"/>
-      <c r="Y19" s="24"/>
-    </row>
-    <row r="20" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y19" s="15"/>
+      <c r="AE19" s="24"/>
+    </row>
+    <row r="20" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>137</v>
       </c>
@@ -2103,9 +2194,10 @@
       <c r="G20" s="15"/>
       <c r="M20" s="15"/>
       <c r="S20" s="15"/>
-      <c r="Y20" s="24"/>
-    </row>
-    <row r="21" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y20" s="15"/>
+      <c r="AE20" s="24"/>
+    </row>
+    <row r="21" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>140</v>
       </c>
@@ -2127,9 +2219,10 @@
       <c r="G21" s="15"/>
       <c r="M21" s="15"/>
       <c r="S21" s="15"/>
-      <c r="Y21" s="24"/>
-    </row>
-    <row r="22" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y21" s="15"/>
+      <c r="AE21" s="24"/>
+    </row>
+    <row r="22" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>143</v>
       </c>
@@ -2193,9 +2286,25 @@
       <c r="X22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="24"/>
-    </row>
-    <row r="23" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE22" s="24"/>
+    </row>
+    <row r="23" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
@@ -2217,9 +2326,10 @@
       <c r="G23" s="15"/>
       <c r="M23" s="15"/>
       <c r="S23" s="15"/>
-      <c r="Y23" s="24"/>
-    </row>
-    <row r="24" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y23" s="15"/>
+      <c r="AE23" s="24"/>
+    </row>
+    <row r="24" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>166</v>
       </c>
@@ -2238,9 +2348,10 @@
       <c r="G24" s="15"/>
       <c r="M24" s="15"/>
       <c r="S24" s="15"/>
-      <c r="Y24" s="24"/>
-    </row>
-    <row r="25" spans="1:25" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y24" s="15"/>
+      <c r="AE24" s="24"/>
+    </row>
+    <row r="25" spans="1:31" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2304,9 +2415,25 @@
       <c r="X25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y25" s="24"/>
-    </row>
-    <row r="26" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE25" s="24"/>
+    </row>
+    <row r="26" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2370,9 +2497,25 @@
       <c r="X26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y26" s="24"/>
-    </row>
-    <row r="27" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE26" s="24"/>
+    </row>
+    <row r="27" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -2436,9 +2579,25 @@
       <c r="X27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y27" s="24"/>
-    </row>
-    <row r="28" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE27" s="24"/>
+    </row>
+    <row r="28" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>145</v>
       </c>
@@ -2502,9 +2661,25 @@
       <c r="X28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y28" s="24"/>
-    </row>
-    <row r="29" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE28" s="24"/>
+    </row>
+    <row r="29" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>260</v>
       </c>
@@ -2526,9 +2701,10 @@
       <c r="G29" s="15"/>
       <c r="M29" s="15"/>
       <c r="S29" s="15"/>
-      <c r="Y29" s="24"/>
-    </row>
-    <row r="30" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y29" s="15"/>
+      <c r="AE29" s="24"/>
+    </row>
+    <row r="30" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>265</v>
       </c>
@@ -2565,9 +2741,10 @@
       <c r="X30" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y30" s="24"/>
-    </row>
-    <row r="31" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y30" s="15"/>
+      <c r="AE30" s="24"/>
+    </row>
+    <row r="31" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -2631,9 +2808,25 @@
       <c r="X31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Y31" s="24"/>
-    </row>
-    <row r="32" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE31" s="24"/>
+    </row>
+    <row r="32" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>168</v>
       </c>
@@ -2655,9 +2848,10 @@
       <c r="G32" s="15"/>
       <c r="M32" s="15"/>
       <c r="S32" s="15"/>
-      <c r="Y32" s="24"/>
-    </row>
-    <row r="33" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y32" s="15"/>
+      <c r="AE32" s="24"/>
+    </row>
+    <row r="33" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>171</v>
       </c>
@@ -2679,9 +2873,10 @@
       <c r="G33" s="15"/>
       <c r="M33" s="15"/>
       <c r="S33" s="15"/>
-      <c r="Y33" s="24"/>
-    </row>
-    <row r="34" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y33" s="15"/>
+      <c r="AE33" s="24"/>
+    </row>
+    <row r="34" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>270</v>
       </c>
@@ -2703,9 +2898,10 @@
       <c r="G34" s="15"/>
       <c r="M34" s="15"/>
       <c r="S34" s="15"/>
-      <c r="Y34" s="1"/>
-    </row>
-    <row r="35" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y34" s="15"/>
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -2727,9 +2923,10 @@
       <c r="G35" s="15"/>
       <c r="M35" s="15"/>
       <c r="S35" s="15"/>
-      <c r="Y35" s="24"/>
-    </row>
-    <row r="36" spans="1:25" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y35" s="15"/>
+      <c r="AE35" s="24"/>
+    </row>
+    <row r="36" spans="1:31" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="20" t="s">
         <v>297</v>
       </c>
@@ -2751,9 +2948,10 @@
       <c r="G36" s="21"/>
       <c r="M36" s="21"/>
       <c r="S36" s="21"/>
-      <c r="Y36" s="1"/>
-    </row>
-    <row r="37" spans="1:25" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y36" s="21"/>
+      <c r="AE36" s="1"/>
+    </row>
+    <row r="37" spans="1:31" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -2775,9 +2973,10 @@
       <c r="G37" s="15"/>
       <c r="M37" s="15"/>
       <c r="S37" s="15"/>
-      <c r="Y37" s="24"/>
-    </row>
-    <row r="38" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y37" s="15"/>
+      <c r="AE37" s="24"/>
+    </row>
+    <row r="38" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -2799,9 +2998,10 @@
       <c r="G38" s="15"/>
       <c r="M38" s="15"/>
       <c r="S38" s="15"/>
-      <c r="Y38" s="24"/>
-    </row>
-    <row r="39" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y38" s="15"/>
+      <c r="AE38" s="24"/>
+    </row>
+    <row r="39" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -2823,9 +3023,10 @@
       <c r="G39" s="15"/>
       <c r="M39" s="15"/>
       <c r="S39" s="15"/>
-      <c r="Y39" s="24"/>
-    </row>
-    <row r="40" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y39" s="15"/>
+      <c r="AE39" s="24"/>
+    </row>
+    <row r="40" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>264</v>
       </c>
@@ -2892,9 +3093,25 @@
       <c r="X40" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y40" s="24"/>
-    </row>
-    <row r="41" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE40" s="24"/>
+    </row>
+    <row r="41" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>174</v>
       </c>
@@ -2958,9 +3175,25 @@
       <c r="X41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y41" s="24"/>
-    </row>
-    <row r="42" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE41" s="24"/>
+    </row>
+    <row r="42" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>45</v>
       </c>
@@ -2982,9 +3215,10 @@
       <c r="G42" s="15"/>
       <c r="M42" s="15"/>
       <c r="S42" s="15"/>
-      <c r="Y42" s="24"/>
-    </row>
-    <row r="43" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y42" s="15"/>
+      <c r="AE42" s="24"/>
+    </row>
+    <row r="43" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>47</v>
       </c>
@@ -3006,9 +3240,10 @@
       <c r="G43" s="15"/>
       <c r="M43" s="15"/>
       <c r="S43" s="15"/>
-      <c r="Y43" s="24"/>
-    </row>
-    <row r="44" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y43" s="15"/>
+      <c r="AE43" s="24"/>
+    </row>
+    <row r="44" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="26" t="s">
         <v>50</v>
       </c>
@@ -3030,9 +3265,10 @@
       <c r="G44" s="15"/>
       <c r="M44" s="15"/>
       <c r="S44" s="15"/>
-      <c r="Y44" s="24"/>
-    </row>
-    <row r="45" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y44" s="15"/>
+      <c r="AE44" s="24"/>
+    </row>
+    <row r="45" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="26"/>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
@@ -3040,9 +3276,10 @@
       <c r="G45" s="15"/>
       <c r="M45" s="15"/>
       <c r="S45" s="15"/>
-      <c r="Y45" s="24"/>
-    </row>
-    <row r="46" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y45" s="15"/>
+      <c r="AE45" s="24"/>
+    </row>
+    <row r="46" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>176</v>
       </c>
@@ -3061,9 +3298,10 @@
       <c r="G46" s="15"/>
       <c r="M46" s="15"/>
       <c r="S46" s="15"/>
-      <c r="Y46" s="24"/>
-    </row>
-    <row r="47" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y46" s="15"/>
+      <c r="AE46" s="24"/>
+    </row>
+    <row r="47" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -3082,9 +3320,10 @@
       <c r="G47" s="15"/>
       <c r="M47" s="15"/>
       <c r="S47" s="15"/>
-      <c r="Y47" s="24"/>
-    </row>
-    <row r="48" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y47" s="15"/>
+      <c r="AE47" s="24"/>
+    </row>
+    <row r="48" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -3106,9 +3345,10 @@
       <c r="G48" s="16"/>
       <c r="M48" s="16"/>
       <c r="S48" s="16"/>
-      <c r="Y48" s="24"/>
-    </row>
-    <row r="49" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y48" s="16"/>
+      <c r="AE48" s="24"/>
+    </row>
+    <row r="49" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>220</v>
       </c>
@@ -3168,9 +3408,25 @@
       <c r="X49" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y49" s="24"/>
-    </row>
-    <row r="50" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y49" s="16"/>
+      <c r="Z49" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC49" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD49" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE49" s="24"/>
+    </row>
+    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="6" t="s">
         <v>179</v>
       </c>
@@ -3192,9 +3448,10 @@
       <c r="G50" s="15"/>
       <c r="M50" s="15"/>
       <c r="S50" s="15"/>
-      <c r="Y50" s="24"/>
-    </row>
-    <row r="51" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y50" s="15"/>
+      <c r="AE50" s="24"/>
+    </row>
+    <row r="51" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="6" t="s">
         <v>181</v>
       </c>
@@ -3216,9 +3473,10 @@
       <c r="G51" s="15"/>
       <c r="M51" s="15"/>
       <c r="S51" s="15"/>
-      <c r="Y51" s="24"/>
-    </row>
-    <row r="52" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y51" s="15"/>
+      <c r="AE51" s="24"/>
+    </row>
+    <row r="52" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -3240,9 +3498,10 @@
       <c r="G52" s="15"/>
       <c r="M52" s="15"/>
       <c r="S52" s="15"/>
-      <c r="Y52" s="24"/>
-    </row>
-    <row r="53" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y52" s="15"/>
+      <c r="AE52" s="24"/>
+    </row>
+    <row r="53" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
@@ -3264,9 +3523,10 @@
       <c r="G53" s="15"/>
       <c r="M53" s="15"/>
       <c r="S53" s="15"/>
-      <c r="Y53" s="24"/>
-    </row>
-    <row r="54" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y53" s="15"/>
+      <c r="AE53" s="24"/>
+    </row>
+    <row r="54" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="6" t="s">
         <v>61</v>
       </c>
@@ -3288,9 +3548,10 @@
       <c r="G54" s="15"/>
       <c r="M54" s="15"/>
       <c r="S54" s="15"/>
-      <c r="Y54" s="24"/>
-    </row>
-    <row r="55" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y54" s="15"/>
+      <c r="AE54" s="24"/>
+    </row>
+    <row r="55" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>184</v>
       </c>
@@ -3312,9 +3573,10 @@
       <c r="G55" s="15"/>
       <c r="M55" s="15"/>
       <c r="S55" s="15"/>
-      <c r="Y55" s="24"/>
-    </row>
-    <row r="56" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y55" s="15"/>
+      <c r="AE55" s="24"/>
+    </row>
+    <row r="56" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>317</v>
       </c>
@@ -3336,9 +3598,10 @@
       <c r="G56" s="15"/>
       <c r="M56" s="15"/>
       <c r="S56" s="15"/>
-      <c r="Y56" s="1"/>
-    </row>
-    <row r="57" spans="1:25" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y56" s="15"/>
+      <c r="AE56" s="1"/>
+    </row>
+    <row r="57" spans="1:31" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="12" t="s">
         <v>303</v>
       </c>
@@ -3371,9 +3634,15 @@
       <c r="R57" s="12"/>
       <c r="S57" s="17"/>
       <c r="T57" s="12"/>
-      <c r="Y57" s="24"/>
-    </row>
-    <row r="58" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y57" s="17"/>
+      <c r="Z57" s="12"/>
+      <c r="AA57" s="12"/>
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="12"/>
+      <c r="AD57" s="12"/>
+      <c r="AE57" s="24"/>
+    </row>
+    <row r="58" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="6" t="s">
         <v>305</v>
       </c>
@@ -3395,9 +3664,10 @@
       <c r="G58" s="15"/>
       <c r="M58" s="15"/>
       <c r="S58" s="15"/>
-      <c r="Y58" s="1"/>
-    </row>
-    <row r="59" spans="1:25" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y58" s="15"/>
+      <c r="AE58" s="1"/>
+    </row>
+    <row r="59" spans="1:31" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="6" t="s">
         <v>309</v>
       </c>
@@ -3429,9 +3699,15 @@
       <c r="Q59" s="19"/>
       <c r="R59" s="19"/>
       <c r="S59" s="15"/>
-      <c r="Y59" s="1"/>
-    </row>
-    <row r="60" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y59" s="15"/>
+      <c r="Z59" s="19"/>
+      <c r="AA59" s="19"/>
+      <c r="AB59" s="19"/>
+      <c r="AC59" s="19"/>
+      <c r="AD59" s="19"/>
+      <c r="AE59" s="1"/>
+    </row>
+    <row r="60" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="6" t="s">
         <v>186</v>
       </c>
@@ -3453,9 +3729,10 @@
       <c r="G60" s="15"/>
       <c r="M60" s="15"/>
       <c r="S60" s="15"/>
-      <c r="Y60" s="24"/>
-    </row>
-    <row r="61" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y60" s="15"/>
+      <c r="AE60" s="24"/>
+    </row>
+    <row r="61" spans="1:31" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="12" t="s">
         <v>240</v>
       </c>
@@ -3492,9 +3769,15 @@
       <c r="V61" s="12"/>
       <c r="W61" s="12"/>
       <c r="X61" s="12"/>
-      <c r="Y61" s="24"/>
-    </row>
-    <row r="62" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y61" s="17"/>
+      <c r="Z61" s="12"/>
+      <c r="AA61" s="12"/>
+      <c r="AB61" s="12"/>
+      <c r="AC61" s="12"/>
+      <c r="AD61" s="12"/>
+      <c r="AE61" s="24"/>
+    </row>
+    <row r="62" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="6" t="s">
         <v>188</v>
       </c>
@@ -3516,9 +3799,10 @@
       <c r="G62" s="15"/>
       <c r="M62" s="15"/>
       <c r="S62" s="15"/>
-      <c r="Y62" s="24"/>
-    </row>
-    <row r="63" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y62" s="15"/>
+      <c r="AE62" s="24"/>
+    </row>
+    <row r="63" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -3540,9 +3824,10 @@
       <c r="G63" s="15"/>
       <c r="M63" s="15"/>
       <c r="S63" s="15"/>
-      <c r="Y63" s="24"/>
-    </row>
-    <row r="64" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y63" s="15"/>
+      <c r="AE63" s="24"/>
+    </row>
+    <row r="64" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="6" t="s">
         <v>65</v>
       </c>
@@ -3564,9 +3849,10 @@
       <c r="G64" s="15"/>
       <c r="M64" s="15"/>
       <c r="S64" s="15"/>
-      <c r="Y64" s="24"/>
-    </row>
-    <row r="65" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y64" s="15"/>
+      <c r="AE64" s="24"/>
+    </row>
+    <row r="65" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>262</v>
       </c>
@@ -3588,9 +3874,10 @@
       <c r="G65" s="15"/>
       <c r="M65" s="15"/>
       <c r="S65" s="15"/>
-      <c r="Y65" s="24"/>
-    </row>
-    <row r="66" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y65" s="15"/>
+      <c r="AE65" s="24"/>
+    </row>
+    <row r="66" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>68</v>
       </c>
@@ -3612,9 +3899,10 @@
       <c r="G66" s="15"/>
       <c r="M66" s="15"/>
       <c r="S66" s="15"/>
-      <c r="Y66" s="24"/>
-    </row>
-    <row r="67" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y66" s="15"/>
+      <c r="AE66" s="24"/>
+    </row>
+    <row r="67" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>70</v>
       </c>
@@ -3636,9 +3924,10 @@
       <c r="G67" s="15"/>
       <c r="M67" s="15"/>
       <c r="S67" s="15"/>
-      <c r="Y67" s="24"/>
-    </row>
-    <row r="68" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y67" s="15"/>
+      <c r="AE67" s="24"/>
+    </row>
+    <row r="68" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>191</v>
       </c>
@@ -3660,9 +3949,10 @@
       <c r="G68" s="15"/>
       <c r="M68" s="15"/>
       <c r="S68" s="15"/>
-      <c r="Y68" s="24"/>
-    </row>
-    <row r="69" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y68" s="15"/>
+      <c r="AE68" s="24"/>
+    </row>
+    <row r="69" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>254</v>
       </c>
@@ -3684,9 +3974,10 @@
       <c r="G69" s="15"/>
       <c r="M69" s="15"/>
       <c r="S69" s="15"/>
-      <c r="Y69" s="24"/>
-    </row>
-    <row r="70" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y69" s="15"/>
+      <c r="AE69" s="24"/>
+    </row>
+    <row r="70" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>72</v>
       </c>
@@ -3750,9 +4041,25 @@
       <c r="X70" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y70" s="24"/>
-    </row>
-    <row r="71" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA70" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB70" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC70" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD70" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE70" s="24"/>
+    </row>
+    <row r="71" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>194</v>
       </c>
@@ -3771,9 +4078,10 @@
       <c r="G71" s="15"/>
       <c r="M71" s="15"/>
       <c r="S71" s="15"/>
-      <c r="Y71" s="24"/>
-    </row>
-    <row r="72" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y71" s="15"/>
+      <c r="AE71" s="24"/>
+    </row>
+    <row r="72" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="6" t="s">
         <v>74</v>
       </c>
@@ -3795,9 +4103,10 @@
       <c r="G72" s="15"/>
       <c r="M72" s="15"/>
       <c r="S72" s="15"/>
-      <c r="Y72" s="24"/>
-    </row>
-    <row r="73" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y72" s="15"/>
+      <c r="AE72" s="24"/>
+    </row>
+    <row r="73" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="20" t="s">
         <v>315</v>
       </c>
@@ -3819,9 +4128,10 @@
       <c r="G73" s="15"/>
       <c r="M73" s="15"/>
       <c r="S73" s="15"/>
-      <c r="Y73" s="1"/>
-    </row>
-    <row r="74" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y73" s="15"/>
+      <c r="AE73" s="1"/>
+    </row>
+    <row r="74" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
         <v>218</v>
       </c>
@@ -3843,9 +4153,10 @@
       <c r="G74" s="15"/>
       <c r="M74" s="15"/>
       <c r="S74" s="15"/>
-      <c r="Y74" s="24"/>
-    </row>
-    <row r="75" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y74" s="15"/>
+      <c r="AE74" s="24"/>
+    </row>
+    <row r="75" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>76</v>
       </c>
@@ -3867,9 +4178,10 @@
       <c r="G75" s="15"/>
       <c r="M75" s="15"/>
       <c r="S75" s="15"/>
-      <c r="Y75" s="24"/>
-    </row>
-    <row r="76" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y75" s="15"/>
+      <c r="AE75" s="24"/>
+    </row>
+    <row r="76" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -3933,9 +4245,25 @@
       <c r="X76" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y76" s="24"/>
-    </row>
-    <row r="77" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y76" s="15"/>
+      <c r="Z76" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA76" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB76" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC76" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD76" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE76" s="24"/>
+    </row>
+    <row r="77" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>80</v>
       </c>
@@ -3957,9 +4285,10 @@
       <c r="G77" s="15"/>
       <c r="M77" s="15"/>
       <c r="S77" s="15"/>
-      <c r="Y77" s="24"/>
-    </row>
-    <row r="78" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y77" s="15"/>
+      <c r="AE77" s="24"/>
+    </row>
+    <row r="78" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="6" t="s">
         <v>83</v>
       </c>
@@ -3981,9 +4310,10 @@
       <c r="G78" s="15"/>
       <c r="M78" s="15"/>
       <c r="S78" s="15"/>
-      <c r="Y78" s="24"/>
-    </row>
-    <row r="79" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y78" s="15"/>
+      <c r="AE78" s="24"/>
+    </row>
+    <row r="79" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>195</v>
       </c>
@@ -4005,9 +4335,10 @@
       <c r="G79" s="15"/>
       <c r="M79" s="15"/>
       <c r="S79" s="15"/>
-      <c r="Y79" s="24"/>
-    </row>
-    <row r="80" spans="1:25" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Y79" s="15"/>
+      <c r="AE79" s="24"/>
+    </row>
+    <row r="80" spans="1:31" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A80" s="6" t="s">
         <v>198</v>
       </c>
@@ -4029,9 +4360,10 @@
       <c r="G80" s="15"/>
       <c r="M80" s="15"/>
       <c r="S80" s="15"/>
-      <c r="Y80" s="24"/>
-    </row>
-    <row r="81" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y80" s="15"/>
+      <c r="AE80" s="24"/>
+    </row>
+    <row r="81" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>85</v>
       </c>
@@ -4095,9 +4427,25 @@
       <c r="X81" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="Y81" s="24"/>
-    </row>
-    <row r="82" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y81" s="15"/>
+      <c r="Z81" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA81" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AB81" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AC81" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD81" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE81" s="24"/>
+    </row>
+    <row r="82" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>87</v>
       </c>
@@ -4119,9 +4467,10 @@
       <c r="G82" s="15"/>
       <c r="M82" s="15"/>
       <c r="S82" s="15"/>
-      <c r="Y82" s="24"/>
-    </row>
-    <row r="83" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y82" s="15"/>
+      <c r="AE82" s="24"/>
+    </row>
+    <row r="83" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="6" t="s">
         <v>91</v>
       </c>
@@ -4143,9 +4492,10 @@
       <c r="G83" s="15"/>
       <c r="M83" s="15"/>
       <c r="S83" s="15"/>
-      <c r="Y83" s="24"/>
-    </row>
-    <row r="84" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y83" s="15"/>
+      <c r="AE83" s="24"/>
+    </row>
+    <row r="84" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="6" t="s">
         <v>148</v>
       </c>
@@ -4167,9 +4517,10 @@
       <c r="G84" s="15"/>
       <c r="M84" s="15"/>
       <c r="S84" s="15"/>
-      <c r="Y84" s="24"/>
-    </row>
-    <row r="85" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y84" s="15"/>
+      <c r="AE84" s="24"/>
+    </row>
+    <row r="85" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="20" t="s">
         <v>322</v>
       </c>
@@ -4212,9 +4563,17 @@
       <c r="X85" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Y85" s="25"/>
-    </row>
-    <row r="86" spans="1:25" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="Y85" s="21"/>
+      <c r="Z85" s="20"/>
+      <c r="AA85" s="20"/>
+      <c r="AB85" s="20"/>
+      <c r="AC85" s="20"/>
+      <c r="AD85" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE85" s="25"/>
+    </row>
+    <row r="86" spans="1:31" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>95</v>
       </c>
@@ -4236,9 +4595,10 @@
       <c r="G86" s="15"/>
       <c r="M86" s="15"/>
       <c r="S86" s="15"/>
-      <c r="Y86" s="24"/>
-    </row>
-    <row r="87" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y86" s="15"/>
+      <c r="AE86" s="24"/>
+    </row>
+    <row r="87" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>225</v>
       </c>
@@ -4298,9 +4658,25 @@
       <c r="X87" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y87" s="24"/>
-    </row>
-    <row r="88" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y87" s="15"/>
+      <c r="Z87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD87" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE87" s="24"/>
+    </row>
+    <row r="88" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
         <v>150</v>
       </c>
@@ -4322,9 +4698,10 @@
       <c r="G88" s="15"/>
       <c r="M88" s="15"/>
       <c r="S88" s="15"/>
-      <c r="Y88" s="24"/>
-    </row>
-    <row r="89" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y88" s="15"/>
+      <c r="AE88" s="24"/>
+    </row>
+    <row r="89" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>98</v>
       </c>
@@ -4346,9 +4723,10 @@
       <c r="G89" s="15"/>
       <c r="M89" s="15"/>
       <c r="S89" s="15"/>
-      <c r="Y89" s="24"/>
-    </row>
-    <row r="90" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y89" s="15"/>
+      <c r="AE89" s="24"/>
+    </row>
+    <row r="90" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>200</v>
       </c>
@@ -4370,9 +4748,10 @@
       <c r="G90" s="15"/>
       <c r="M90" s="15"/>
       <c r="S90" s="15"/>
-      <c r="Y90" s="24"/>
-    </row>
-    <row r="91" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y90" s="15"/>
+      <c r="AE90" s="24"/>
+    </row>
+    <row r="91" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>248</v>
       </c>
@@ -4394,9 +4773,10 @@
       <c r="G91" s="15"/>
       <c r="M91" s="15"/>
       <c r="S91" s="15"/>
-      <c r="Y91" s="24"/>
-    </row>
-    <row r="92" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y91" s="15"/>
+      <c r="AE91" s="24"/>
+    </row>
+    <row r="92" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>221</v>
       </c>
@@ -4414,9 +4794,10 @@
       <c r="G92" s="15"/>
       <c r="M92" s="15"/>
       <c r="S92" s="15"/>
-      <c r="Y92" s="24"/>
-    </row>
-    <row r="93" spans="1:25" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Y92" s="15"/>
+      <c r="AE92" s="24"/>
+    </row>
+    <row r="93" spans="1:31" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>100</v>
       </c>
@@ -4438,9 +4819,10 @@
       <c r="G93" s="15"/>
       <c r="M93" s="15"/>
       <c r="S93" s="15"/>
-      <c r="Y93" s="24"/>
-    </row>
-    <row r="94" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y93" s="15"/>
+      <c r="AE93" s="24"/>
+    </row>
+    <row r="94" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>299</v>
       </c>
@@ -4462,9 +4844,10 @@
       <c r="G94" s="15"/>
       <c r="M94" s="15"/>
       <c r="S94" s="15"/>
-      <c r="Y94" s="1"/>
-    </row>
-    <row r="95" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y94" s="15"/>
+      <c r="AE94" s="1"/>
+    </row>
+    <row r="95" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>102</v>
       </c>
@@ -4486,9 +4869,10 @@
       <c r="G95" s="15"/>
       <c r="M95" s="15"/>
       <c r="S95" s="15"/>
-      <c r="Y95" s="24"/>
-    </row>
-    <row r="96" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y95" s="15"/>
+      <c r="AE95" s="24"/>
+    </row>
+    <row r="96" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>104</v>
       </c>
@@ -4510,9 +4894,10 @@
       <c r="G96" s="15"/>
       <c r="M96" s="15"/>
       <c r="S96" s="15"/>
-      <c r="Y96" s="24"/>
-    </row>
-    <row r="97" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y96" s="15"/>
+      <c r="AE96" s="24"/>
+    </row>
+    <row r="97" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>203</v>
       </c>
@@ -4531,9 +4916,10 @@
       <c r="G97" s="15"/>
       <c r="M97" s="15"/>
       <c r="S97" s="15"/>
-      <c r="Y97" s="24"/>
-    </row>
-    <row r="98" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y97" s="15"/>
+      <c r="AE97" s="24"/>
+    </row>
+    <row r="98" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>106</v>
       </c>
@@ -4555,9 +4941,10 @@
       <c r="G98" s="15"/>
       <c r="M98" s="15"/>
       <c r="S98" s="15"/>
-      <c r="Y98" s="24"/>
-    </row>
-    <row r="99" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y98" s="15"/>
+      <c r="AE98" s="24"/>
+    </row>
+    <row r="99" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>110</v>
       </c>
@@ -4621,9 +5008,25 @@
       <c r="X99" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y99" s="24"/>
-    </row>
-    <row r="100" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y99" s="15"/>
+      <c r="Z99" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA99" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB99" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC99" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD99" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE99" s="24"/>
+    </row>
+    <row r="100" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="6" t="s">
         <v>112</v>
       </c>
@@ -4645,9 +5048,10 @@
       <c r="G100" s="15"/>
       <c r="M100" s="15"/>
       <c r="S100" s="15"/>
-      <c r="Y100" s="24"/>
-    </row>
-    <row r="101" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y100" s="15"/>
+      <c r="AE100" s="24"/>
+    </row>
+    <row r="101" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="6" t="s">
         <v>114</v>
       </c>
@@ -4669,9 +5073,10 @@
       <c r="G101" s="15"/>
       <c r="M101" s="15"/>
       <c r="S101" s="15"/>
-      <c r="Y101" s="24"/>
-    </row>
-    <row r="102" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y101" s="15"/>
+      <c r="AE101" s="24"/>
+    </row>
+    <row r="102" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="6" t="s">
         <v>116</v>
       </c>
@@ -4693,9 +5098,10 @@
       <c r="G102" s="15"/>
       <c r="M102" s="15"/>
       <c r="S102" s="15"/>
-      <c r="Y102" s="24"/>
-    </row>
-    <row r="103" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y102" s="15"/>
+      <c r="AE102" s="24"/>
+    </row>
+    <row r="103" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>118</v>
       </c>
@@ -4759,9 +5165,25 @@
       <c r="X103" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y103" s="24"/>
-    </row>
-    <row r="104" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y103" s="15"/>
+      <c r="Z103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD103" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE103" s="24"/>
+    </row>
+    <row r="104" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>120</v>
       </c>
@@ -4825,9 +5247,25 @@
       <c r="X104" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y104" s="24"/>
-    </row>
-    <row r="105" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y104" s="15"/>
+      <c r="Z104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE104" s="24"/>
+    </row>
+    <row r="105" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>122</v>
       </c>
@@ -4891,9 +5329,25 @@
       <c r="X105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y105" s="24"/>
-    </row>
-    <row r="106" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y105" s="15"/>
+      <c r="Z105" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE105" s="24"/>
+    </row>
+    <row r="106" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>152</v>
       </c>
@@ -4920,9 +5374,10 @@
       <c r="L106"/>
       <c r="M106" s="15"/>
       <c r="S106" s="15"/>
-      <c r="Y106" s="24"/>
-    </row>
-    <row r="107" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y106" s="15"/>
+      <c r="AE106" s="24"/>
+    </row>
+    <row r="107" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>301</v>
       </c>
@@ -4959,9 +5414,15 @@
       <c r="V107"/>
       <c r="W107"/>
       <c r="X107"/>
-      <c r="Y107" s="1"/>
-    </row>
-    <row r="108" spans="1:25" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y107" s="15"/>
+      <c r="Z107"/>
+      <c r="AA107"/>
+      <c r="AB107"/>
+      <c r="AC107"/>
+      <c r="AD107"/>
+      <c r="AE107" s="1"/>
+    </row>
+    <row r="108" spans="1:31" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="6" t="s">
         <v>124</v>
       </c>
@@ -4983,9 +5444,10 @@
       <c r="G108" s="15"/>
       <c r="M108" s="15"/>
       <c r="S108" s="15"/>
-      <c r="Y108" s="1"/>
-    </row>
-    <row r="109" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y108" s="15"/>
+      <c r="AE108" s="1"/>
+    </row>
+    <row r="109" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>127</v>
       </c>
@@ -5049,9 +5511,25 @@
       <c r="X109" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y109" s="1"/>
-    </row>
-    <row r="110" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y109" s="15"/>
+      <c r="Z109" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE109" s="1"/>
+    </row>
+    <row r="110" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>239</v>
       </c>
@@ -5115,9 +5593,25 @@
       <c r="X110" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y110" s="1"/>
-    </row>
-    <row r="111" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y110" s="15"/>
+      <c r="Z110" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE110" s="1"/>
+    </row>
+    <row r="111" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>130</v>
       </c>
@@ -5139,9 +5633,10 @@
       <c r="G111" s="15"/>
       <c r="M111" s="15"/>
       <c r="S111" s="15"/>
-      <c r="Y111" s="1"/>
-    </row>
-    <row r="112" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Y111" s="15"/>
+      <c r="AE111" s="1"/>
+    </row>
+    <row r="112" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>313</v>
       </c>
@@ -5205,9 +5700,25 @@
       <c r="X112" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y112" s="1"/>
-    </row>
-    <row r="113" spans="1:25" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="Y112" s="15"/>
+      <c r="Z112" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA112" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB112" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC112" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD112" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE112" s="1"/>
+    </row>
+    <row r="113" spans="1:31" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>257</v>
       </c>
@@ -5229,9 +5740,10 @@
       <c r="G113" s="15"/>
       <c r="M113" s="15"/>
       <c r="S113" s="15"/>
-      <c r="Y113" s="1"/>
-    </row>
-    <row r="114" spans="1:25" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Y113" s="15"/>
+      <c r="AE113" s="1"/>
+    </row>
+    <row r="114" spans="1:31" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>132</v>
       </c>
@@ -5253,73 +5765,74 @@
       <c r="G114" s="15"/>
       <c r="M114" s="15"/>
       <c r="S114" s="15"/>
-      <c r="Y114" s="1"/>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y115" s="24"/>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y116" s="24"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y117" s="24"/>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y118" s="24"/>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y119" s="24"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y120" s="24"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y121" s="24"/>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y122" s="24"/>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y123" s="24"/>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y124" s="24"/>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y125" s="24"/>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y126" s="24"/>
-    </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y127" s="24"/>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="Y128" s="24"/>
-    </row>
-    <row r="129" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y129" s="24"/>
-    </row>
-    <row r="130" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y130" s="24"/>
-    </row>
-    <row r="131" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y131" s="24"/>
-    </row>
-    <row r="132" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y132" s="24"/>
-    </row>
-    <row r="133" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y133" s="24"/>
-    </row>
-    <row r="134" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y134" s="24"/>
-    </row>
-    <row r="135" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y135" s="24"/>
-    </row>
-    <row r="136" spans="25:25" x14ac:dyDescent="0.4">
-      <c r="Y136" s="24"/>
+      <c r="Y114" s="15"/>
+      <c r="AE114" s="1"/>
+    </row>
+    <row r="115" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE115" s="24"/>
+    </row>
+    <row r="116" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE116" s="24"/>
+    </row>
+    <row r="117" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE117" s="24"/>
+    </row>
+    <row r="118" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE118" s="24"/>
+    </row>
+    <row r="119" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE119" s="24"/>
+    </row>
+    <row r="120" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE120" s="24"/>
+    </row>
+    <row r="121" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE121" s="24"/>
+    </row>
+    <row r="122" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE122" s="24"/>
+    </row>
+    <row r="123" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE123" s="24"/>
+    </row>
+    <row r="124" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE124" s="24"/>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE125" s="24"/>
+    </row>
+    <row r="126" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE126" s="24"/>
+    </row>
+    <row r="127" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE127" s="24"/>
+    </row>
+    <row r="128" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="AE128" s="24"/>
+    </row>
+    <row r="129" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE129" s="24"/>
+    </row>
+    <row r="130" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE130" s="24"/>
+    </row>
+    <row r="131" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE131" s="24"/>
+    </row>
+    <row r="132" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE132" s="24"/>
+    </row>
+    <row r="133" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE133" s="24"/>
+    </row>
+    <row r="134" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE134" s="24"/>
+    </row>
+    <row r="135" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE135" s="24"/>
+    </row>
+    <row r="136" spans="31:31" x14ac:dyDescent="0.4">
+      <c r="AE136" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
IHW: Correcties op validatie van MIM model
Zie #255
Hier is beschreven dat het type van een "GEGEVENSGROEP" attribuut
beperkt is, en in ider geval geen  "REFERENTIELIJST" kan zijn.

Ook is een interface acceptabel als type.

Minor, uitbreiding van validatie en MIM format XML schema
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\IHW\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F741839-994A-45D3-8B2B-4F37E70B1F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ED0D4B-E897-4162-910E-AF87FD31559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="330">
   <si>
     <t>Name</t>
   </si>
@@ -1010,6 +1010,12 @@
   </si>
   <si>
     <t>LOGICAL</t>
+  </si>
+  <si>
+    <t>createeatoolbox</t>
+  </si>
+  <si>
+    <t>Should an EA toolbox be generated?</t>
   </si>
 </sst>
 </file>
@@ -1507,13 +1513,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T140"/>
+  <dimension ref="A1:T141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H103" sqref="H103:R103"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2245,104 +2251,61 @@
       <c r="E26" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F26" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G26" s="15"/>
       <c r="H26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="M26" s="15"/>
       <c r="N26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="S26" s="15"/>
       <c r="T26" s="24"/>
     </row>
     <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>328</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>32</v>
+        <v>329</v>
       </c>
       <c r="D27" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="M27" s="15"/>
       <c r="N27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="S27" s="15"/>
-      <c r="T27" s="24"/>
     </row>
     <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -2352,7 +2315,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>4</v>
@@ -2361,14 +2324,14 @@
         <v>4</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="M28" s="15"/>
       <c r="N28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>4</v>
@@ -2377,20 +2340,20 @@
         <v>4</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="S28" s="15"/>
       <c r="T28" s="24"/>
     </row>
     <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>260</v>
+        <v>145</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>261</v>
+        <v>146</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>
@@ -2398,23 +2361,50 @@
       <c r="E29" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G29" s="15"/>
+      <c r="H29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="M29" s="15"/>
+      <c r="N29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="S29" s="15"/>
       <c r="T29" s="24"/>
     </row>
     <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
@@ -2423,22 +2413,22 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>300</v>
+        <v>16</v>
       </c>
       <c r="G30" s="15"/>
       <c r="M30" s="15"/>
       <c r="S30" s="15"/>
       <c r="T30" s="24"/>
     </row>
-    <row r="31" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>265</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>36</v>
+        <v>266</v>
       </c>
       <c r="D31" s="2" t="b">
         <v>0</v>
@@ -2446,50 +2436,23 @@
       <c r="E31" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>300</v>
+      </c>
       <c r="G31" s="15"/>
-      <c r="H31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="M31" s="15"/>
-      <c r="N31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="S31" s="15"/>
       <c r="T31" s="24"/>
     </row>
     <row r="32" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>169</v>
+        <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
@@ -2497,23 +2460,50 @@
       <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G32" s="15"/>
+      <c r="H32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="M32" s="15"/>
+      <c r="N32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="S32" s="15"/>
       <c r="T32" s="24"/>
     </row>
-    <row r="33" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2522,22 +2512,22 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>269</v>
+        <v>10</v>
       </c>
       <c r="G33" s="15"/>
       <c r="M33" s="15"/>
       <c r="S33" s="15"/>
       <c r="T33" s="24"/>
     </row>
-    <row r="34" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>270</v>
+        <v>171</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>271</v>
+        <v>172</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>272</v>
+        <v>173</v>
       </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
@@ -2546,22 +2536,22 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G34" s="15"/>
       <c r="M34" s="15"/>
       <c r="S34" s="15"/>
-      <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T34" s="24"/>
+    </row>
+    <row r="35" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>37</v>
+        <v>270</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>5</v>
+        <v>271</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>38</v>
+        <v>272</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
@@ -2570,76 +2560,76 @@
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>16</v>
+        <v>273</v>
       </c>
       <c r="G35" s="15"/>
       <c r="M35" s="15"/>
       <c r="S35" s="15"/>
-      <c r="T35" s="24"/>
-    </row>
-    <row r="36" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="20" t="s">
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="24"/>
+    </row>
+    <row r="37" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B37" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C37" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="D36" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="1"/>
-    </row>
-    <row r="37" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+      <c r="D37" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="1"/>
+    </row>
+    <row r="38" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="24"/>
-    </row>
-    <row r="38" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>16</v>
@@ -2649,21 +2639,21 @@
       <c r="S38" s="15"/>
       <c r="T38" s="24"/>
     </row>
-    <row r="39" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>16</v>
@@ -2675,13 +2665,13 @@
     </row>
     <row r="40" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>264</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>267</v>
+        <v>44</v>
       </c>
       <c r="D40" s="2" t="b">
         <v>0</v>
@@ -2690,127 +2680,127 @@
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>300</v>
+        <v>16</v>
       </c>
       <c r="G40" s="15"/>
-      <c r="H40" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="M40" s="15"/>
-      <c r="N40" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="S40" s="15"/>
       <c r="T40" s="24"/>
     </row>
     <row r="41" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>175</v>
+        <v>267</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="2" t="s">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="M41" s="15"/>
       <c r="N41" s="2" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="S41" s="15"/>
       <c r="T41" s="24"/>
     </row>
-    <row r="42" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A42" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="6" t="s">
+    <row r="42" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>16</v>
+      <c r="C42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G42" s="15"/>
+      <c r="H42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="M42" s="15"/>
+      <c r="N42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="S42" s="15"/>
       <c r="T42" s="24"/>
     </row>
-    <row r="43" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D43" s="6" t="b">
         <v>1</v>
@@ -2819,31 +2809,31 @@
         <v>0</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>219</v>
+        <v>16</v>
       </c>
       <c r="G43" s="15"/>
       <c r="M43" s="15"/>
       <c r="S43" s="15"/>
       <c r="T43" s="24"/>
     </row>
-    <row r="44" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>16</v>
+    <row r="44" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="G44" s="15"/>
       <c r="M44" s="15"/>
@@ -2851,162 +2841,162 @@
       <c r="T44" s="24"/>
     </row>
     <row r="45" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
+      <c r="A45" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G45" s="15"/>
       <c r="M45" s="15"/>
       <c r="S45" s="15"/>
       <c r="T45" s="24"/>
     </row>
-    <row r="46" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="46" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
       <c r="G46" s="15"/>
       <c r="M46" s="15"/>
       <c r="S46" s="15"/>
       <c r="T46" s="24"/>
     </row>
-    <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
+        <v>177</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>53</v>
+        <v>178</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="15"/>
       <c r="M47" s="15"/>
       <c r="S47" s="15"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="24"/>
+    </row>
+    <row r="49" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" s="5" t="s">
+      <c r="D49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="G48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="S48" s="16"/>
-      <c r="T48" s="24"/>
-    </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="G49" s="16"/>
-      <c r="H49" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M49" s="15"/>
-      <c r="N49" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R49" s="2" t="s">
-        <v>327</v>
-      </c>
+      <c r="M49" s="16"/>
       <c r="S49" s="16"/>
       <c r="T49" s="24"/>
     </row>
-    <row r="50" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="M50" s="15"/>
+      <c r="N50" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="S50" s="16"/>
+      <c r="T50" s="24"/>
+    </row>
+    <row r="51" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D50" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="S50" s="15"/>
-      <c r="T50" s="24"/>
-    </row>
-    <row r="51" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A51" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>183</v>
-      </c>
       <c r="D51" s="6" t="b">
         <v>0</v>
       </c>
@@ -3014,31 +3004,31 @@
         <v>1</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>209</v>
+        <v>4</v>
       </c>
       <c r="G51" s="15"/>
       <c r="M51" s="15"/>
       <c r="S51" s="15"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>16</v>
+    <row r="52" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D52" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>209</v>
       </c>
       <c r="G52" s="15"/>
       <c r="M52" s="15"/>
@@ -3047,13 +3037,13 @@
     </row>
     <row r="53" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D53" s="2" t="b">
         <v>0</v>
@@ -3069,23 +3059,23 @@
       <c r="S53" s="15"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="6" t="s">
+    <row r="54" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D54" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="6" t="s">
+      <c r="C54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="15"/>
@@ -3093,23 +3083,23 @@
       <c r="S54" s="15"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B55" s="2" t="s">
+    <row r="55" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="C55" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="15"/>
@@ -3117,15 +3107,15 @@
       <c r="S55" s="15"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
-        <v>306</v>
+        <v>184</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>307</v>
+        <v>185</v>
       </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
@@ -3134,229 +3124,229 @@
         <v>1</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G56" s="15"/>
       <c r="M56" s="15"/>
       <c r="S56" s="15"/>
-      <c r="T56" s="1"/>
-    </row>
-    <row r="57" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="12" t="s">
+      <c r="T56" s="24"/>
+    </row>
+    <row r="57" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="S57" s="15"/>
+      <c r="T57" s="1"/>
+    </row>
+    <row r="58" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B58" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C58" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="D57" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="12" t="s">
+      <c r="D58" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="12"/>
-      <c r="S57" s="17"/>
-      <c r="T57" s="24"/>
-    </row>
-    <row r="58" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="6" t="s">
+      <c r="G58" s="17"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="24"/>
+    </row>
+    <row r="59" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="D58" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="6" t="s">
+      <c r="D59" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="G58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="S58" s="15"/>
-      <c r="T58" s="1"/>
-    </row>
-    <row r="59" spans="1:20" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="D59" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>312</v>
-      </c>
       <c r="G59" s="15"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
       <c r="M59" s="15"/>
-      <c r="N59" s="19"/>
-      <c r="O59" s="19"/>
-      <c r="P59" s="19"/>
-      <c r="Q59" s="19"/>
-      <c r="R59" s="19"/>
       <c r="S59" s="15"/>
       <c r="T59" s="1"/>
     </row>
-    <row r="60" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:20" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A60" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D60" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="G60" s="15"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="19"/>
+      <c r="O60" s="19"/>
+      <c r="P60" s="19"/>
+      <c r="Q60" s="19"/>
+      <c r="R60" s="19"/>
+      <c r="S60" s="15"/>
+      <c r="T60" s="1"/>
+    </row>
+    <row r="61" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B61" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="6" t="s">
+      <c r="D61" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="G60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="24"/>
-    </row>
-    <row r="61" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="12" t="s">
+      <c r="G61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="S61" s="15"/>
+      <c r="T61" s="24"/>
+    </row>
+    <row r="62" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B62" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C62" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="12" t="s">
+      <c r="D62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-      <c r="R61" s="12"/>
-      <c r="S61" s="17"/>
-      <c r="T61" s="24"/>
-    </row>
-    <row r="62" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="6" t="s">
+      <c r="G62" s="17"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="17"/>
+      <c r="T62" s="24"/>
+    </row>
+    <row r="63" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B63" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="6" t="s">
+      <c r="D63" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="G62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="S62" s="15"/>
-      <c r="T62" s="24"/>
-    </row>
-    <row r="63" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G63" s="15"/>
       <c r="M63" s="15"/>
       <c r="S63" s="15"/>
       <c r="T63" s="24"/>
     </row>
-    <row r="64" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D64" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>219</v>
+    <row r="64" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="G64" s="15"/>
       <c r="M64" s="15"/>
@@ -3364,62 +3354,62 @@
       <c r="T64" s="24"/>
     </row>
     <row r="65" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>262</v>
-      </c>
-      <c r="B65" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" t="s">
-        <v>263</v>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>227</v>
+      <c r="A65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="G65" s="15"/>
       <c r="M65" s="15"/>
       <c r="S65" s="15"/>
       <c r="T65" s="24"/>
     </row>
-    <row r="66" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>210</v>
+    <row r="66" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>262</v>
+      </c>
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" t="s">
+        <v>263</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>227</v>
       </c>
       <c r="G66" s="15"/>
       <c r="M66" s="15"/>
       <c r="S66" s="15"/>
       <c r="T66" s="24"/>
     </row>
-    <row r="67" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
@@ -3428,31 +3418,31 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>285</v>
+        <v>210</v>
       </c>
       <c r="G67" s="15"/>
       <c r="M67" s="15"/>
       <c r="S67" s="15"/>
       <c r="T67" s="24"/>
     </row>
-    <row r="68" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
       <c r="G68" s="15"/>
       <c r="M68" s="15"/>
@@ -3461,13 +3451,13 @@
     </row>
     <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>254</v>
+        <v>191</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>256</v>
+        <v>193</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
@@ -3476,52 +3466,52 @@
         <v>1</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>255</v>
+        <v>208</v>
       </c>
       <c r="G69" s="15"/>
       <c r="M69" s="15"/>
       <c r="S69" s="15"/>
       <c r="T69" s="24"/>
     </row>
-    <row r="70" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>72</v>
+        <v>254</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>73</v>
+        <v>256</v>
       </c>
       <c r="D70" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="G70" s="15"/>
       <c r="M70" s="15"/>
       <c r="S70" s="15"/>
       <c r="T70" s="24"/>
     </row>
-    <row r="71" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>315</v>
+        <v>72</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>316</v>
+        <v>73</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>317</v>
+        <v>0</v>
       </c>
       <c r="G71" s="15"/>
       <c r="M71" s="15"/>
@@ -3530,13 +3520,13 @@
     </row>
     <row r="72" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>241</v>
+        <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D72" s="2" t="b">
         <v>0</v>
@@ -3545,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G72" s="15"/>
       <c r="M72" s="15"/>
@@ -3554,13 +3544,13 @@
     </row>
     <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>10</v>
+        <v>241</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
@@ -3568,50 +3558,23 @@
       <c r="E73" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F73" s="2" t="s">
+        <v>324</v>
+      </c>
       <c r="G73" s="15"/>
-      <c r="H73" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="M73" s="15"/>
-      <c r="N73" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P73" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q73" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R73" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="S73" s="15"/>
       <c r="T73" s="24"/>
     </row>
     <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>241</v>
+        <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3620,19 +3583,49 @@
         <v>1</v>
       </c>
       <c r="G74" s="15"/>
+      <c r="H74" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="M74" s="15"/>
+      <c r="N74" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="P74" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q74" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="R74" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="S74" s="15"/>
       <c r="T74" s="24"/>
     </row>
     <row r="75" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>194</v>
+        <v>322</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>241</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3645,312 +3638,309 @@
       <c r="S75" s="15"/>
       <c r="T75" s="24"/>
     </row>
-    <row r="76" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D76" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>4</v>
+    <row r="76" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G76" s="15"/>
       <c r="M76" s="15"/>
       <c r="S76" s="15"/>
       <c r="T76" s="24"/>
     </row>
-    <row r="77" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="B77" s="20" t="s">
+    <row r="77" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="D77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="C77" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G77" s="15"/>
       <c r="M77" s="15"/>
       <c r="S77" s="15"/>
-      <c r="T77" s="1"/>
-    </row>
-    <row r="78" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B78" s="2" t="s">
+      <c r="T77" s="24"/>
+    </row>
+    <row r="78" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B78" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>230</v>
+      <c r="C78" s="20" t="s">
+        <v>305</v>
       </c>
       <c r="D78" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G78" s="15"/>
       <c r="M78" s="15"/>
       <c r="S78" s="15"/>
-      <c r="T78" s="24"/>
+      <c r="T78" s="1"/>
     </row>
     <row r="79" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>76</v>
+        <v>218</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>77</v>
+        <v>230</v>
       </c>
       <c r="D79" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G79" s="15"/>
       <c r="M79" s="15"/>
       <c r="S79" s="15"/>
       <c r="T79" s="24"/>
     </row>
-    <row r="80" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D80" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G80" s="15"/>
       <c r="M80" s="15"/>
       <c r="S80" s="15"/>
       <c r="T80" s="24"/>
     </row>
-    <row r="81" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D81" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="G81" s="15"/>
       <c r="M81" s="15"/>
       <c r="S81" s="15"/>
       <c r="T81" s="24"/>
     </row>
-    <row r="82" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D82" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>280</v>
+    <row r="82" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="G82" s="15"/>
       <c r="M82" s="15"/>
       <c r="S82" s="15"/>
       <c r="T82" s="24"/>
     </row>
-    <row r="83" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>19</v>
+    <row r="83" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>280</v>
       </c>
       <c r="G83" s="15"/>
       <c r="M83" s="15"/>
       <c r="S83" s="15"/>
       <c r="T83" s="24"/>
     </row>
-    <row r="84" spans="1:20" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A84" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D84" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>211</v>
+    <row r="84" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G84" s="15"/>
       <c r="M84" s="15"/>
       <c r="S84" s="15"/>
       <c r="T84" s="24"/>
     </row>
-    <row r="85" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>0</v>
+    <row r="85" spans="1:20" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A85" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D85" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="G85" s="15"/>
-      <c r="H85" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L85" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="M85" s="15"/>
-      <c r="N85" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O85" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P85" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q85" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R85" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="S85" s="15"/>
       <c r="T85" s="24"/>
     </row>
     <row r="86" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G86" s="15"/>
+      <c r="H86" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="M86" s="15"/>
+      <c r="N86" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="P86" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q86" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="R86" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="S86" s="15"/>
       <c r="T86" s="24"/>
     </row>
-    <row r="87" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D87" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>92</v>
+    <row r="87" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="G87" s="15"/>
       <c r="M87" s="15"/>
@@ -3959,22 +3949,22 @@
     </row>
     <row r="88" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="6" t="s">
-        <v>148</v>
+        <v>91</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D88" s="6" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="G88" s="15"/>
       <c r="M88" s="15"/>
@@ -3982,180 +3972,180 @@
       <c r="T88" s="24"/>
     </row>
     <row r="89" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="20" t="s">
+      <c r="A89" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D89" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="15"/>
+      <c r="M89" s="15"/>
+      <c r="S89" s="15"/>
+      <c r="T89" s="24"/>
+    </row>
+    <row r="90" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B90" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C90" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="D89" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="15"/>
-      <c r="H89" s="20"/>
-      <c r="I89" s="20"/>
-      <c r="J89" s="20"/>
-      <c r="K89" s="20"/>
-      <c r="L89" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="M89" s="21"/>
-      <c r="N89" s="20"/>
-      <c r="O89" s="20"/>
-      <c r="P89" s="20"/>
-      <c r="Q89" s="20"/>
-      <c r="R89" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="S89" s="21"/>
-      <c r="T89" s="25"/>
-    </row>
-    <row r="90" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
+      <c r="D90" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="15"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="20"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M90" s="21"/>
+      <c r="N90" s="20"/>
+      <c r="O90" s="20"/>
+      <c r="P90" s="20"/>
+      <c r="Q90" s="20"/>
+      <c r="R90" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="S90" s="21"/>
+      <c r="T90" s="25"/>
+    </row>
+    <row r="91" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" s="2" t="s">
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G90" s="15"/>
-      <c r="M90" s="15"/>
-      <c r="S90" s="15"/>
-      <c r="T90" s="24"/>
-    </row>
-    <row r="91" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="G91" s="15"/>
-      <c r="H91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L91" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="M91" s="15"/>
-      <c r="N91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R91" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="S91" s="15"/>
       <c r="T91" s="24"/>
     </row>
     <row r="92" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
       <c r="D92" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F92" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G92" s="15"/>
+      <c r="H92" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="M92" s="15"/>
+      <c r="N92" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O92" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R92" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="S92" s="15"/>
       <c r="T92" s="24"/>
     </row>
     <row r="93" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="D93" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>268</v>
+        <v>4</v>
       </c>
       <c r="G93" s="15"/>
       <c r="M93" s="15"/>
       <c r="S93" s="15"/>
       <c r="T93" s="24"/>
     </row>
-    <row r="94" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>200</v>
+        <v>98</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>201</v>
+        <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
       <c r="D94" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="G94" s="15"/>
       <c r="M94" s="15"/>
@@ -4164,13 +4154,13 @@
     </row>
     <row r="95" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>248</v>
+        <v>200</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
@@ -4178,115 +4168,115 @@
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="5" t="s">
-        <v>251</v>
+      <c r="F95" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="G95" s="15"/>
       <c r="M95" s="15"/>
       <c r="S95" s="15"/>
       <c r="T95" s="24"/>
     </row>
-    <row r="96" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+        <v>248</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>280</v>
+      <c r="F96" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="G96" s="15"/>
       <c r="M96" s="15"/>
       <c r="S96" s="15"/>
       <c r="T96" s="24"/>
     </row>
-    <row r="97" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
       <c r="D97" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>16</v>
+        <v>280</v>
       </c>
       <c r="G97" s="15"/>
       <c r="M97" s="15"/>
       <c r="S97" s="15"/>
       <c r="T97" s="24"/>
     </row>
-    <row r="98" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
-        <v>288</v>
-      </c>
-      <c r="B98" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" t="s">
-        <v>289</v>
-      </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" t="s">
-        <v>280</v>
+    <row r="98" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G98" s="15"/>
       <c r="M98" s="15"/>
       <c r="S98" s="15"/>
-      <c r="T98" s="1"/>
-    </row>
-    <row r="99" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>212</v>
+      <c r="T98" s="24"/>
+    </row>
+    <row r="99" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>288</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" t="s">
+        <v>289</v>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>280</v>
       </c>
       <c r="G99" s="15"/>
       <c r="M99" s="15"/>
       <c r="S99" s="15"/>
-      <c r="T99" s="24"/>
+      <c r="T99" s="1"/>
     </row>
     <row r="100" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D100" s="2" t="b">
         <v>0</v>
@@ -4294,29 +4284,32 @@
       <c r="E100" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F100" s="2" t="s">
-        <v>16</v>
+      <c r="F100" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="G100" s="15"/>
       <c r="M100" s="15"/>
       <c r="S100" s="15"/>
       <c r="T100" s="24"/>
     </row>
-    <row r="101" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E101" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G101" s="15"/>
       <c r="M101" s="15"/>
@@ -4325,37 +4318,34 @@
     </row>
     <row r="102" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="G102" s="15"/>
       <c r="M102" s="15"/>
       <c r="S102" s="15"/>
       <c r="T102" s="24"/>
     </row>
-    <row r="103" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D103" s="2" t="b">
         <v>1</v>
@@ -4363,74 +4353,74 @@
       <c r="E103" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F103" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G103" s="15"/>
-      <c r="H103" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="M103" s="15"/>
-      <c r="N103" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O103" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P103" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q103" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R103" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="S103" s="15"/>
       <c r="T103" s="24"/>
     </row>
-    <row r="104" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D104" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>219</v>
+    <row r="104" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G104" s="15"/>
+      <c r="H104" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="M104" s="15"/>
+      <c r="N104" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="O104" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="P104" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q104" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="R104" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="S104" s="15"/>
       <c r="T104" s="24"/>
     </row>
     <row r="105" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D105" s="6" t="b">
         <v>1</v>
@@ -4448,91 +4438,64 @@
     </row>
     <row r="106" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D106" s="6" t="b">
         <v>1</v>
       </c>
       <c r="E106" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>16</v>
+        <v>219</v>
       </c>
       <c r="G106" s="15"/>
       <c r="M106" s="15"/>
       <c r="S106" s="15"/>
       <c r="T106" s="24"/>
     </row>
-    <row r="107" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B107" s="2" t="s">
+    <row r="107" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
+      <c r="C107" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D107" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G107" s="15"/>
-      <c r="H107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="M107" s="15"/>
-      <c r="N107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R107" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="S107" s="15"/>
       <c r="T107" s="24"/>
     </row>
     <row r="108" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D108" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108" s="2" t="b">
         <v>1</v>
@@ -4574,23 +4537,23 @@
     </row>
     <row r="109" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D109" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G109" s="15"/>
       <c r="H109" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>4</v>
@@ -4606,7 +4569,7 @@
       </c>
       <c r="M109" s="15"/>
       <c r="N109" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O109" s="2" t="s">
         <v>4</v>
@@ -4623,15 +4586,15 @@
       <c r="S109" s="15"/>
       <c r="T109" s="24"/>
     </row>
-    <row r="110" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="D110" s="2" t="b">
         <v>0</v>
@@ -4639,36 +4602,58 @@
       <c r="E110" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F110" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G110" s="15"/>
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="J110"/>
-      <c r="K110"/>
-      <c r="L110"/>
+      <c r="H110" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="M110" s="15"/>
+      <c r="N110" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R110" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="S110" s="15"/>
       <c r="T110" s="24"/>
     </row>
-    <row r="111" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>290</v>
-      </c>
-      <c r="B111" t="s">
+    <row r="111" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C111" t="s">
-        <v>291</v>
-      </c>
-      <c r="D111" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
+      <c r="C111" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G111" s="15"/>
@@ -4678,98 +4663,76 @@
       <c r="K111"/>
       <c r="L111"/>
       <c r="M111" s="15"/>
-      <c r="N111"/>
-      <c r="O111"/>
-      <c r="P111"/>
-      <c r="Q111"/>
-      <c r="R111"/>
       <c r="S111" s="15"/>
-      <c r="T111" s="1"/>
-    </row>
-    <row r="112" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D112" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>16</v>
+      <c r="T111" s="24"/>
+    </row>
+    <row r="112" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>290</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>291</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>4</v>
       </c>
       <c r="G112" s="15"/>
+      <c r="H112"/>
+      <c r="I112"/>
+      <c r="J112"/>
+      <c r="K112"/>
+      <c r="L112"/>
       <c r="M112" s="15"/>
+      <c r="N112"/>
+      <c r="O112"/>
+      <c r="P112"/>
+      <c r="Q112"/>
+      <c r="R112"/>
       <c r="S112" s="15"/>
       <c r="T112" s="1"/>
     </row>
-    <row r="113" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="2" t="b">
-        <v>1</v>
+    <row r="113" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A113" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D113" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G113" s="15"/>
-      <c r="H113" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L113" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="M113" s="15"/>
-      <c r="N113" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R113" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="S113" s="15"/>
       <c r="T113" s="1"/>
     </row>
     <row r="114" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>239</v>
+        <v>127</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D114" s="2" t="b">
         <v>1</v>
@@ -4814,88 +4777,88 @@
     </row>
     <row r="115" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D115" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E115" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>280</v>
+        <v>1</v>
       </c>
       <c r="G115" s="15"/>
+      <c r="H115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="M115" s="15"/>
+      <c r="N115" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R115" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="S115" s="15"/>
       <c r="T115" s="1"/>
     </row>
     <row r="116" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>302</v>
+        <v>130</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>303</v>
+        <v>131</v>
       </c>
       <c r="D116" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E116" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="G116" s="15"/>
-      <c r="H116" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="J116" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L116" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="M116" s="15"/>
-      <c r="N116" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O116" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P116" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q116" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R116" s="2" t="s">
-        <v>327</v>
-      </c>
       <c r="S116" s="15"/>
       <c r="T116" s="1"/>
     </row>
-    <row r="117" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="D117" s="2" t="b">
         <v>1</v>
@@ -4903,40 +4866,88 @@
       <c r="E117" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="G117" s="15"/>
+      <c r="H117" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>326</v>
+      </c>
       <c r="M117" s="15"/>
+      <c r="N117" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="P117" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="R117" s="2" t="s">
+        <v>327</v>
+      </c>
       <c r="S117" s="15"/>
       <c r="T117" s="1"/>
     </row>
-    <row r="118" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>132</v>
+        <v>257</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>134</v>
+        <v>258</v>
       </c>
       <c r="D118" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="G118" s="15"/>
       <c r="M118" s="15"/>
       <c r="S118" s="15"/>
       <c r="T118" s="1"/>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T119" s="24"/>
+    <row r="119" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A119" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G119" s="15"/>
+      <c r="M119" s="15"/>
+      <c r="S119" s="15"/>
+      <c r="T119" s="1"/>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.4">
       <c r="T120" s="24"/>
@@ -5000,6 +5011,9 @@
     </row>
     <row r="140" spans="20:20" x14ac:dyDescent="0.4">
       <c r="T140" s="24"/>
+    </row>
+    <row r="141" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T141" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5007,14 +5021,14 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F59" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F60" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F20" r:id="rId3" xr:uid="{8E59784E-ED1C-4906-9E7A-BA97BE01137B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IHW: alleen nog conceptuele en logische modellen
De aansluiting bij VNGR SIM/UGM/BSM is verlaten.

Improvement.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\IHW\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07ED0D4B-E897-4162-910E-AF87FD31559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4082420B-F934-411A-9A54-B5145CBA8BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="321">
   <si>
     <t>Name</t>
   </si>
@@ -643,9 +643,6 @@
     <t>Yes if warnings should be suppressed in documentation</t>
   </si>
   <si>
-    <t>release</t>
-  </si>
-  <si>
     <t>00000000</t>
   </si>
   <si>
@@ -850,24 +847,6 @@
     <t>respec</t>
   </si>
   <si>
-    <t>SIM: opleveren</t>
-  </si>
-  <si>
-    <t>SIM: docrelease</t>
-  </si>
-  <si>
-    <t>UGM: minimum</t>
-  </si>
-  <si>
-    <t>UGM: uitgebreid</t>
-  </si>
-  <si>
-    <t>UGM: opleveren</t>
-  </si>
-  <si>
-    <t>UGM: docrelease</t>
-  </si>
-  <si>
     <t>IHW</t>
   </si>
   <si>
@@ -877,12 +856,6 @@
     <t>ihw</t>
   </si>
   <si>
-    <t>SIM: minimum</t>
-  </si>
-  <si>
-    <t>SIM: uitgebreid</t>
-  </si>
-  <si>
     <t>IHW_GEOSTANDAARDEN</t>
   </si>
   <si>
@@ -952,12 +925,6 @@
     <t>Should a full respec version be generated along with the catalog?</t>
   </si>
   <si>
-    <t>SIM: regtest</t>
-  </si>
-  <si>
-    <t>UGM: regtest</t>
-  </si>
-  <si>
     <t>regression</t>
   </si>
   <si>
@@ -1016,6 +983,12 @@
   </si>
   <si>
     <t>Should an EA toolbox be generated?</t>
+  </si>
+  <si>
+    <t>CONCEPTUAL: uitgebreid</t>
+  </si>
+  <si>
+    <t>LOGICAL: uitgebreid</t>
   </si>
 </sst>
 </file>
@@ -1513,13 +1486,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T141"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1531,21 +1504,14 @@
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
     <col min="7" max="7" width="5.4609375" style="18" customWidth="1"/>
-    <col min="8" max="9" width="14.765625" customWidth="1"/>
-    <col min="10" max="10" width="14.3046875" customWidth="1"/>
-    <col min="11" max="11" width="15.765625" customWidth="1"/>
-    <col min="12" max="12" width="12.84375" customWidth="1"/>
-    <col min="13" max="13" width="5.4609375" style="18" customWidth="1"/>
-    <col min="14" max="14" width="16.15234375" customWidth="1"/>
-    <col min="15" max="15" width="16.07421875" customWidth="1"/>
-    <col min="16" max="16" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.765625" customWidth="1"/>
-    <col min="18" max="18" width="13.15234375" customWidth="1"/>
-    <col min="19" max="19" width="5.4609375" style="18" customWidth="1"/>
-    <col min="20" max="20" width="27.3046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.53515625" customWidth="1"/>
+    <col min="9" max="9" width="5.4609375" style="18" customWidth="1"/>
+    <col min="10" max="10" width="20.61328125" customWidth="1"/>
+    <col min="11" max="11" width="5.4609375" style="18" customWidth="1"/>
+    <col min="12" max="12" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1556,89 +1522,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>215</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>253</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="I1" s="13"/>
       <c r="J1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+        <v>252</v>
+      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="14"/>
       <c r="H2" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>284</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="I2" s="14"/>
       <c r="J2" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="23"/>
-    </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+        <v>320</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -1655,11 +1573,11 @@
         <v>1</v>
       </c>
       <c r="G3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="24"/>
-    </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="24"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1679,11 +1597,11 @@
         <v>4</v>
       </c>
       <c r="G4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="24"/>
-    </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1703,11 +1621,11 @@
         <v>4</v>
       </c>
       <c r="G5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="24"/>
-    </row>
-    <row r="6" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="24"/>
+    </row>
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>157</v>
       </c>
@@ -1724,11 +1642,11 @@
         <v>1</v>
       </c>
       <c r="G6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="24"/>
-    </row>
-    <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="24"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -1745,21 +1663,21 @@
         <v>1</v>
       </c>
       <c r="G7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="24"/>
-    </row>
-    <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="G8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="24"/>
-    </row>
-    <row r="9" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="24"/>
+    </row>
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>160</v>
       </c>
@@ -1779,11 +1697,11 @@
         <v>16</v>
       </c>
       <c r="G9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="24"/>
-    </row>
-    <row r="10" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1803,11 +1721,11 @@
         <v>4</v>
       </c>
       <c r="G10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="24"/>
-    </row>
-    <row r="11" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="24"/>
+    </row>
+    <row r="11" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>162</v>
       </c>
@@ -1824,11 +1742,11 @@
         <v>1</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="24"/>
-    </row>
-    <row r="12" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="24"/>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>135</v>
       </c>
@@ -1848,35 +1766,35 @@
         <v>4</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="24"/>
-    </row>
-    <row r="13" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="G13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="24"/>
-    </row>
-    <row r="14" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="24"/>
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1896,11 +1814,11 @@
         <v>16</v>
       </c>
       <c r="G14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="24"/>
-    </row>
-    <row r="15" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="24"/>
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1916,42 +1834,15 @@
       <c r="E15" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S15" s="15"/>
-      <c r="T15" s="24"/>
-    </row>
-    <row r="16" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="24"/>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1971,37 +1862,37 @@
         <v>10</v>
       </c>
       <c r="G16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="24"/>
-    </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="24"/>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="24"/>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="G17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="24"/>
-    </row>
-    <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2012,14 +1903,14 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="24"/>
-    </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="24"/>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -2036,11 +1927,11 @@
         <v>1</v>
       </c>
       <c r="G19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="24"/>
-    </row>
-    <row r="20" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="24"/>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>137</v>
       </c>
@@ -2057,14 +1948,14 @@
         <v>1</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="G20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="24"/>
-    </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>140</v>
       </c>
@@ -2081,14 +1972,14 @@
         <v>1</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="G21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="24"/>
-    </row>
-    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="24"/>
+    </row>
+    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>143</v>
       </c>
@@ -2104,42 +1995,15 @@
       <c r="E22" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G22" s="15"/>
-      <c r="H22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M22" s="15"/>
-      <c r="N22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S22" s="15"/>
-      <c r="T22" s="24"/>
-    </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="24"/>
+    </row>
+    <row r="23" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
@@ -2159,11 +2023,11 @@
         <v>16</v>
       </c>
       <c r="G23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="24"/>
-    </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>166</v>
       </c>
@@ -2180,11 +2044,11 @@
         <v>1</v>
       </c>
       <c r="G24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="24"/>
-    </row>
-    <row r="25" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2200,42 +2064,15 @@
       <c r="E25" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F25" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G25" s="15"/>
-      <c r="H25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="15"/>
-      <c r="N25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S25" s="15"/>
-      <c r="T25" s="24"/>
-    </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="24"/>
+    </row>
+    <row r="26" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2255,25 +2092,19 @@
         <v>4</v>
       </c>
       <c r="G26" s="15"/>
-      <c r="H26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" s="15"/>
-      <c r="N26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="15"/>
-      <c r="T26" s="24"/>
-    </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="24"/>
+    </row>
+    <row r="27" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
@@ -2285,16 +2116,11 @@
         <v>4</v>
       </c>
       <c r="G27" s="15"/>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="15"/>
-      <c r="N27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S27" s="15"/>
-    </row>
-    <row r="28" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="24"/>
+    </row>
+    <row r="28" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2310,42 +2136,15 @@
       <c r="E28" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F28" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="15"/>
-      <c r="H28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="15"/>
-      <c r="N28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="15"/>
-      <c r="T28" s="24"/>
-    </row>
-    <row r="29" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="24"/>
+    </row>
+    <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>145</v>
       </c>
@@ -2361,50 +2160,23 @@
       <c r="E29" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G29" s="15"/>
-      <c r="H29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M29" s="15"/>
-      <c r="N29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S29" s="15"/>
-      <c r="T29" s="24"/>
-    </row>
-    <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="24"/>
+    </row>
+    <row r="30" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
@@ -2416,19 +2188,19 @@
         <v>16</v>
       </c>
       <c r="G30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="24"/>
-    </row>
-    <row r="31" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="24"/>
+    </row>
+    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D31" s="2" t="b">
         <v>0</v>
@@ -2437,14 +2209,14 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="G31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="24"/>
-    </row>
-    <row r="32" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="24"/>
+    </row>
+    <row r="32" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2464,38 +2236,14 @@
       <c r="H32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="I32" s="15"/>
       <c r="J32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M32" s="15"/>
-      <c r="N32" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S32" s="15"/>
-      <c r="T32" s="24"/>
-    </row>
-    <row r="33" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K32" s="15"/>
+      <c r="L32" s="24"/>
+    </row>
+    <row r="33" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>168</v>
       </c>
@@ -2515,11 +2263,11 @@
         <v>10</v>
       </c>
       <c r="G33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="24"/>
-    </row>
-    <row r="34" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="24"/>
+    </row>
+    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>171</v>
       </c>
@@ -2536,38 +2284,38 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="24"/>
+    </row>
+    <row r="35" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="24"/>
-    </row>
-    <row r="35" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="G35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="1"/>
-    </row>
-    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -2587,19 +2335,19 @@
         <v>16</v>
       </c>
       <c r="G36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="24"/>
-    </row>
-    <row r="37" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="24"/>
+    </row>
+    <row r="37" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="20" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D37" s="20" t="b">
         <v>0</v>
@@ -2611,11 +2359,11 @@
         <v>16</v>
       </c>
       <c r="G37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="1"/>
-    </row>
-    <row r="38" spans="1:20" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
@@ -2635,11 +2383,11 @@
         <v>16</v>
       </c>
       <c r="G38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="24"/>
-    </row>
-    <row r="39" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="24"/>
+    </row>
+    <row r="39" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -2659,11 +2407,11 @@
         <v>16</v>
       </c>
       <c r="G39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="24"/>
-    </row>
-    <row r="40" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="24"/>
+    </row>
+    <row r="40" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -2683,19 +2431,19 @@
         <v>16</v>
       </c>
       <c r="G40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="24"/>
-    </row>
-    <row r="41" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="24"/>
+    </row>
+    <row r="41" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
@@ -2704,44 +2452,20 @@
         <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="I41" s="15"/>
       <c r="J41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M41" s="15"/>
-      <c r="N41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S41" s="15"/>
-      <c r="T41" s="24"/>
-    </row>
-    <row r="42" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>316</v>
+      </c>
+      <c r="K41" s="15"/>
+      <c r="L41" s="24"/>
+    </row>
+    <row r="42" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>174</v>
       </c>
@@ -2757,42 +2481,15 @@
       <c r="E42" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F42" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G42" s="15"/>
-      <c r="H42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M42" s="15"/>
-      <c r="N42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S42" s="15"/>
-      <c r="T42" s="24"/>
-    </row>
-    <row r="43" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="24"/>
+    </row>
+    <row r="43" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>45</v>
       </c>
@@ -2812,11 +2509,11 @@
         <v>16</v>
       </c>
       <c r="G43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="24"/>
-    </row>
-    <row r="44" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="24"/>
+    </row>
+    <row r="44" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>47</v>
       </c>
@@ -2833,14 +2530,14 @@
         <v>0</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="24"/>
-    </row>
-    <row r="45" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="24"/>
+    </row>
+    <row r="45" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="26" t="s">
         <v>50</v>
       </c>
@@ -2860,21 +2557,21 @@
         <v>16</v>
       </c>
       <c r="G45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="24"/>
-    </row>
-    <row r="46" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="24"/>
+    </row>
+    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="26"/>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
       <c r="D46" s="26"/>
       <c r="G46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="S46" s="15"/>
-      <c r="T46" s="24"/>
-    </row>
-    <row r="47" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="24"/>
+    </row>
+    <row r="47" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>176</v>
       </c>
@@ -2891,11 +2588,11 @@
         <v>0</v>
       </c>
       <c r="G47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="24"/>
-    </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="24"/>
+    </row>
+    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -2912,11 +2609,11 @@
         <v>1</v>
       </c>
       <c r="G48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="24"/>
-    </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="24"/>
+    </row>
+    <row r="49" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2933,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="S49" s="16"/>
-      <c r="T49" s="24"/>
-    </row>
-    <row r="50" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="24"/>
+    </row>
+    <row r="50" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -2954,40 +2651,16 @@
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="I50" s="15"/>
       <c r="J50" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M50" s="15"/>
-      <c r="N50" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q50" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R50" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S50" s="16"/>
-      <c r="T50" s="24"/>
-    </row>
-    <row r="51" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+        <v>316</v>
+      </c>
+      <c r="K50" s="16"/>
+      <c r="L50" s="24"/>
+    </row>
+    <row r="51" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="6" t="s">
         <v>179</v>
       </c>
@@ -3007,11 +2680,11 @@
         <v>4</v>
       </c>
       <c r="G51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="24"/>
-    </row>
-    <row r="52" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="24"/>
+    </row>
+    <row r="52" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A52" s="6" t="s">
         <v>181</v>
       </c>
@@ -3028,14 +2701,14 @@
         <v>1</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="S52" s="15"/>
-      <c r="T52" s="24"/>
-    </row>
-    <row r="53" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="24"/>
+    </row>
+    <row r="53" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -3055,11 +2728,11 @@
         <v>16</v>
       </c>
       <c r="G53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="24"/>
-    </row>
-    <row r="54" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="24"/>
+    </row>
+    <row r="54" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -3079,11 +2752,11 @@
         <v>16</v>
       </c>
       <c r="G54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="S54" s="15"/>
-      <c r="T54" s="24"/>
-    </row>
-    <row r="55" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="24"/>
+    </row>
+    <row r="55" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="6" t="s">
         <v>61</v>
       </c>
@@ -3103,11 +2776,11 @@
         <v>16</v>
       </c>
       <c r="G55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="S55" s="15"/>
-      <c r="T55" s="24"/>
-    </row>
-    <row r="56" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="24"/>
+    </row>
+    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>184</v>
       </c>
@@ -3127,19 +2800,19 @@
         <v>16</v>
       </c>
       <c r="G56" s="15"/>
-      <c r="M56" s="15"/>
-      <c r="S56" s="15"/>
-      <c r="T56" s="24"/>
-    </row>
-    <row r="57" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="24"/>
+    </row>
+    <row r="57" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D57" s="2" t="b">
         <v>0</v>
@@ -3151,19 +2824,19 @@
         <v>4</v>
       </c>
       <c r="G57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="S57" s="15"/>
-      <c r="T57" s="1"/>
-    </row>
-    <row r="58" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A58" s="12" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D58" s="12" t="b">
         <v>0</v>
@@ -3172,32 +2845,24 @@
         <v>1</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="G58" s="17"/>
       <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
+      <c r="I58" s="17"/>
       <c r="J58" s="12"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="12"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="12"/>
-      <c r="S58" s="17"/>
-      <c r="T58" s="24"/>
-    </row>
-    <row r="59" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K58" s="17"/>
+      <c r="L58" s="24"/>
+    </row>
+    <row r="59" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="6" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D59" s="6" t="b">
         <v>0</v>
@@ -3206,22 +2871,22 @@
         <v>1</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="G59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="S59" s="15"/>
-      <c r="T59" s="1"/>
-    </row>
-    <row r="60" spans="1:20" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="1"/>
+    </row>
+    <row r="60" spans="1:12" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A60" s="6" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>89</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D60" s="6" t="b">
         <v>0</v>
@@ -3230,24 +2895,16 @@
         <v>1</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="I60" s="15"/>
       <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="19"/>
-      <c r="P60" s="19"/>
-      <c r="Q60" s="19"/>
-      <c r="R60" s="19"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="1"/>
-    </row>
-    <row r="61" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K60" s="15"/>
+      <c r="L60" s="1"/>
+    </row>
+    <row r="61" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="6" t="s">
         <v>186</v>
       </c>
@@ -3264,48 +2921,40 @@
         <v>1</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="G61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="S61" s="15"/>
-      <c r="T61" s="24"/>
-    </row>
-    <row r="62" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="24"/>
+    </row>
+    <row r="62" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="C62" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="D62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="D62" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>243</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
+      <c r="I62" s="17"/>
       <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="12"/>
-      <c r="S62" s="17"/>
-      <c r="T62" s="24"/>
-    </row>
-    <row r="63" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K62" s="17"/>
+      <c r="L62" s="24"/>
+    </row>
+    <row r="63" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" s="6" t="s">
         <v>188</v>
       </c>
@@ -3325,11 +2974,11 @@
         <v>19</v>
       </c>
       <c r="G63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="S63" s="15"/>
-      <c r="T63" s="24"/>
-    </row>
-    <row r="64" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="24"/>
+    </row>
+    <row r="64" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
@@ -3346,14 +2995,14 @@
         <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="24"/>
-    </row>
-    <row r="65" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="24"/>
+    </row>
+    <row r="65" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="6" t="s">
         <v>65</v>
       </c>
@@ -3370,22 +3019,22 @@
         <v>0</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="24"/>
-    </row>
-    <row r="66" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="24"/>
+    </row>
+    <row r="66" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B66" t="s">
         <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -3394,14 +3043,14 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="24"/>
-    </row>
-    <row r="67" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="24"/>
+    </row>
+    <row r="67" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
@@ -3418,14 +3067,14 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="24"/>
-    </row>
-    <row r="68" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="24"/>
+    </row>
+    <row r="68" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
@@ -3442,14 +3091,14 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="G68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="24"/>
-    </row>
-    <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="24"/>
+    </row>
+    <row r="69" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -3466,38 +3115,38 @@
         <v>1</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="24"/>
-    </row>
-    <row r="70" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="24"/>
+    </row>
+    <row r="70" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="G70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="24"/>
-    </row>
-    <row r="71" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="24"/>
+    </row>
+    <row r="71" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
@@ -3514,19 +3163,19 @@
         <v>0</v>
       </c>
       <c r="G71" s="15"/>
-      <c r="M71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="24"/>
-    </row>
-    <row r="72" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="24"/>
+    </row>
+    <row r="72" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D72" s="2" t="b">
         <v>0</v>
@@ -3535,22 +3184,22 @@
         <v>1</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="G72" s="15"/>
-      <c r="M72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="24"/>
-    </row>
-    <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="24"/>
+    </row>
+    <row r="73" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
@@ -3559,22 +3208,22 @@
         <v>1</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="G73" s="15"/>
-      <c r="M73" s="15"/>
-      <c r="S73" s="15"/>
-      <c r="T73" s="24"/>
-    </row>
-    <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="24"/>
+    </row>
+    <row r="74" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3584,48 +3233,24 @@
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="I74" s="15"/>
       <c r="J74" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M74" s="15"/>
-      <c r="N74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S74" s="15"/>
-      <c r="T74" s="24"/>
-    </row>
-    <row r="75" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>316</v>
+      </c>
+      <c r="K74" s="15"/>
+      <c r="L74" s="24"/>
+    </row>
+    <row r="75" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3634,11 +3259,11 @@
         <v>1</v>
       </c>
       <c r="G75" s="15"/>
-      <c r="M75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="24"/>
-    </row>
-    <row r="76" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="24"/>
+    </row>
+    <row r="76" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>194</v>
       </c>
@@ -3646,7 +3271,7 @@
         <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -3655,11 +3280,11 @@
         <v>1</v>
       </c>
       <c r="G76" s="15"/>
-      <c r="M76" s="15"/>
-      <c r="S76" s="15"/>
-      <c r="T76" s="24"/>
-    </row>
-    <row r="77" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="24"/>
+    </row>
+    <row r="77" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="6" t="s">
         <v>74</v>
       </c>
@@ -3679,19 +3304,19 @@
         <v>4</v>
       </c>
       <c r="G77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="S77" s="15"/>
-      <c r="T77" s="24"/>
-    </row>
-    <row r="78" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="24"/>
+    </row>
+    <row r="78" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="20" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
@@ -3703,19 +3328,19 @@
         <v>4</v>
       </c>
       <c r="G78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="1"/>
-    </row>
-    <row r="79" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="1"/>
+    </row>
+    <row r="79" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D79" s="2" t="b">
         <v>1</v>
@@ -3727,11 +3352,11 @@
         <v>16</v>
       </c>
       <c r="G79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="24"/>
-    </row>
-    <row r="80" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="24"/>
+    </row>
+    <row r="80" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
@@ -3751,11 +3376,11 @@
         <v>4</v>
       </c>
       <c r="G80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="24"/>
-    </row>
-    <row r="81" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="24"/>
+    </row>
+    <row r="81" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -3772,11 +3397,11 @@
         <v>0</v>
       </c>
       <c r="G81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="24"/>
-    </row>
-    <row r="82" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="24"/>
+    </row>
+    <row r="82" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
@@ -3793,14 +3418,14 @@
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="G82" s="15"/>
-      <c r="M82" s="15"/>
-      <c r="S82" s="15"/>
-      <c r="T82" s="24"/>
-    </row>
-    <row r="83" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="24"/>
+    </row>
+    <row r="83" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A83" s="6" t="s">
         <v>83</v>
       </c>
@@ -3817,14 +3442,14 @@
         <v>0</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G83" s="15"/>
-      <c r="M83" s="15"/>
-      <c r="S83" s="15"/>
-      <c r="T83" s="24"/>
-    </row>
-    <row r="84" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="24"/>
+    </row>
+    <row r="84" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>195</v>
       </c>
@@ -3844,11 +3469,11 @@
         <v>19</v>
       </c>
       <c r="G84" s="15"/>
-      <c r="M84" s="15"/>
-      <c r="S84" s="15"/>
-      <c r="T84" s="24"/>
-    </row>
-    <row r="85" spans="1:20" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="I84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="24"/>
+    </row>
+    <row r="85" spans="1:12" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A85" s="6" t="s">
         <v>198</v>
       </c>
@@ -3865,14 +3490,14 @@
         <v>1</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G85" s="15"/>
-      <c r="M85" s="15"/>
-      <c r="S85" s="15"/>
-      <c r="T85" s="24"/>
-    </row>
-    <row r="86" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="24"/>
+    </row>
+    <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
@@ -3890,40 +3515,16 @@
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="I86" s="15"/>
       <c r="J86" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M86" s="15"/>
-      <c r="N86" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O86" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P86" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q86" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R86" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S86" s="15"/>
-      <c r="T86" s="24"/>
-    </row>
-    <row r="87" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>316</v>
+      </c>
+      <c r="K86" s="15"/>
+      <c r="L86" s="24"/>
+    </row>
+    <row r="87" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
@@ -3943,11 +3544,11 @@
         <v>88</v>
       </c>
       <c r="G87" s="15"/>
-      <c r="M87" s="15"/>
-      <c r="S87" s="15"/>
-      <c r="T87" s="24"/>
-    </row>
-    <row r="88" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="24"/>
+    </row>
+    <row r="88" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="6" t="s">
         <v>91</v>
       </c>
@@ -3967,11 +3568,11 @@
         <v>92</v>
       </c>
       <c r="G88" s="15"/>
-      <c r="M88" s="15"/>
-      <c r="S88" s="15"/>
-      <c r="T88" s="24"/>
-    </row>
-    <row r="89" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="24"/>
+    </row>
+    <row r="89" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="6" t="s">
         <v>148</v>
       </c>
@@ -3991,19 +3592,19 @@
         <v>16</v>
       </c>
       <c r="G89" s="15"/>
-      <c r="M89" s="15"/>
-      <c r="S89" s="15"/>
-      <c r="T89" s="24"/>
-    </row>
-    <row r="90" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="24"/>
+    </row>
+    <row r="90" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="20" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B90" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="D90" s="20" t="b">
         <v>0</v>
@@ -4016,24 +3617,12 @@
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="20"/>
-      <c r="I90" s="20"/>
+      <c r="I90" s="21"/>
       <c r="J90" s="20"/>
-      <c r="K90" s="20"/>
-      <c r="L90" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="M90" s="21"/>
-      <c r="N90" s="20"/>
-      <c r="O90" s="20"/>
-      <c r="P90" s="20"/>
-      <c r="Q90" s="20"/>
-      <c r="R90" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="S90" s="21"/>
-      <c r="T90" s="25"/>
-    </row>
-    <row r="91" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="K90" s="21"/>
+      <c r="L90" s="25"/>
+    </row>
+    <row r="91" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -4053,13 +3642,13 @@
         <v>96</v>
       </c>
       <c r="G91" s="15"/>
-      <c r="M91" s="15"/>
-      <c r="S91" s="15"/>
-      <c r="T91" s="24"/>
-    </row>
-    <row r="92" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I91" s="15"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="24"/>
+    </row>
+    <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -4069,42 +3658,15 @@
       <c r="E92" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F92" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G92" s="15"/>
-      <c r="H92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M92" s="15"/>
-      <c r="N92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S92" s="15"/>
-      <c r="T92" s="24"/>
-    </row>
-    <row r="93" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="24"/>
+    </row>
+    <row r="93" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>150</v>
       </c>
@@ -4124,11 +3686,11 @@
         <v>4</v>
       </c>
       <c r="G93" s="15"/>
-      <c r="M93" s="15"/>
-      <c r="S93" s="15"/>
-      <c r="T93" s="24"/>
-    </row>
-    <row r="94" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I93" s="15"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="24"/>
+    </row>
+    <row r="94" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>98</v>
       </c>
@@ -4145,14 +3707,14 @@
         <v>0</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G94" s="15"/>
-      <c r="M94" s="15"/>
-      <c r="S94" s="15"/>
-      <c r="T94" s="24"/>
-    </row>
-    <row r="95" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I94" s="15"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="24"/>
+    </row>
+    <row r="95" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
         <v>200</v>
       </c>
@@ -4169,40 +3731,40 @@
         <v>1</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G95" s="15"/>
-      <c r="M95" s="15"/>
-      <c r="S95" s="15"/>
-      <c r="T95" s="24"/>
-    </row>
-    <row r="96" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="24"/>
+    </row>
+    <row r="96" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>251</v>
-      </c>
       <c r="G96" s="15"/>
-      <c r="M96" s="15"/>
-      <c r="S96" s="15"/>
-      <c r="T96" s="24"/>
-    </row>
-    <row r="97" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I96" s="15"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="24"/>
+    </row>
+    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -4213,14 +3775,14 @@
         <v>1</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G97" s="15"/>
-      <c r="M97" s="15"/>
-      <c r="S97" s="15"/>
-      <c r="T97" s="24"/>
-    </row>
-    <row r="98" spans="1:20" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I97" s="15"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="24"/>
+    </row>
+    <row r="98" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
@@ -4240,19 +3802,19 @@
         <v>16</v>
       </c>
       <c r="G98" s="15"/>
-      <c r="M98" s="15"/>
-      <c r="S98" s="15"/>
-      <c r="T98" s="24"/>
-    </row>
-    <row r="99" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="24"/>
+    </row>
+    <row r="99" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D99" t="b">
         <v>1</v>
@@ -4261,14 +3823,14 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G99" s="15"/>
-      <c r="M99" s="15"/>
-      <c r="S99" s="15"/>
-      <c r="T99" s="1"/>
-    </row>
-    <row r="100" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I99" s="15"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="1"/>
+    </row>
+    <row r="100" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>102</v>
       </c>
@@ -4285,14 +3847,14 @@
         <v>1</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G100" s="15"/>
-      <c r="M100" s="15"/>
-      <c r="S100" s="15"/>
-      <c r="T100" s="24"/>
-    </row>
-    <row r="101" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I100" s="15"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="24"/>
+    </row>
+    <row r="101" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
@@ -4312,11 +3874,11 @@
         <v>16</v>
       </c>
       <c r="G101" s="15"/>
-      <c r="M101" s="15"/>
-      <c r="S101" s="15"/>
-      <c r="T101" s="24"/>
-    </row>
-    <row r="102" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I101" s="15"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="24"/>
+    </row>
+    <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
         <v>203</v>
       </c>
@@ -4333,11 +3895,11 @@
         <v>1</v>
       </c>
       <c r="G102" s="15"/>
-      <c r="M102" s="15"/>
-      <c r="S102" s="15"/>
-      <c r="T102" s="24"/>
-    </row>
-    <row r="103" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I102" s="15"/>
+      <c r="K102" s="15"/>
+      <c r="L102" s="24"/>
+    </row>
+    <row r="103" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
@@ -4357,11 +3919,11 @@
         <v>107</v>
       </c>
       <c r="G103" s="15"/>
-      <c r="M103" s="15"/>
-      <c r="S103" s="15"/>
-      <c r="T103" s="24"/>
-    </row>
-    <row r="104" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I103" s="15"/>
+      <c r="K103" s="15"/>
+      <c r="L103" s="24"/>
+    </row>
+    <row r="104" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>110</v>
       </c>
@@ -4379,40 +3941,16 @@
       </c>
       <c r="G104" s="15"/>
       <c r="H104" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="I104" s="15"/>
       <c r="J104" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L104" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M104" s="15"/>
-      <c r="N104" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O104" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P104" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q104" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R104" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S104" s="15"/>
-      <c r="T104" s="24"/>
-    </row>
-    <row r="105" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+        <v>316</v>
+      </c>
+      <c r="K104" s="15"/>
+      <c r="L104" s="24"/>
+    </row>
+    <row r="105" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="6" t="s">
         <v>112</v>
       </c>
@@ -4429,14 +3967,14 @@
         <v>0</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G105" s="15"/>
-      <c r="M105" s="15"/>
-      <c r="S105" s="15"/>
-      <c r="T105" s="24"/>
-    </row>
-    <row r="106" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I105" s="15"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="24"/>
+    </row>
+    <row r="106" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="6" t="s">
         <v>114</v>
       </c>
@@ -4453,14 +3991,14 @@
         <v>0</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G106" s="15"/>
-      <c r="M106" s="15"/>
-      <c r="S106" s="15"/>
-      <c r="T106" s="24"/>
-    </row>
-    <row r="107" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I106" s="15"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="24"/>
+    </row>
+    <row r="107" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="6" t="s">
         <v>116</v>
       </c>
@@ -4480,11 +4018,11 @@
         <v>16</v>
       </c>
       <c r="G107" s="15"/>
-      <c r="M107" s="15"/>
-      <c r="S107" s="15"/>
-      <c r="T107" s="24"/>
-    </row>
-    <row r="108" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I107" s="15"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="24"/>
+    </row>
+    <row r="108" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>118</v>
       </c>
@@ -4500,42 +4038,15 @@
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F108" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G108" s="15"/>
-      <c r="H108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M108" s="15"/>
-      <c r="N108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S108" s="15"/>
-      <c r="T108" s="24"/>
-    </row>
-    <row r="109" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I108" s="15"/>
+      <c r="K108" s="15"/>
+      <c r="L108" s="24"/>
+    </row>
+    <row r="109" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
         <v>120</v>
       </c>
@@ -4551,42 +4062,15 @@
       <c r="E109" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F109" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G109" s="15"/>
-      <c r="H109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M109" s="15"/>
-      <c r="N109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S109" s="15"/>
-      <c r="T109" s="24"/>
-    </row>
-    <row r="110" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I109" s="15"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="24"/>
+    </row>
+    <row r="110" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>122</v>
       </c>
@@ -4602,42 +4086,15 @@
       <c r="E110" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F110" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G110" s="15"/>
-      <c r="H110" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M110" s="15"/>
-      <c r="N110" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S110" s="15"/>
-      <c r="T110" s="24"/>
-    </row>
-    <row r="111" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I110" s="15"/>
+      <c r="K110" s="15"/>
+      <c r="L110" s="24"/>
+    </row>
+    <row r="111" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>152</v>
       </c>
@@ -4658,23 +4115,19 @@
       </c>
       <c r="G111" s="15"/>
       <c r="H111"/>
-      <c r="I111"/>
-      <c r="J111"/>
-      <c r="K111"/>
-      <c r="L111"/>
-      <c r="M111" s="15"/>
-      <c r="S111" s="15"/>
-      <c r="T111" s="24"/>
-    </row>
-    <row r="112" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I111" s="15"/>
+      <c r="K111" s="15"/>
+      <c r="L111" s="24"/>
+    </row>
+    <row r="112" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B112" t="s">
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="D112" t="b">
         <v>0</v>
@@ -4687,20 +4140,12 @@
       </c>
       <c r="G112" s="15"/>
       <c r="H112"/>
-      <c r="I112"/>
+      <c r="I112" s="15"/>
       <c r="J112"/>
-      <c r="K112"/>
-      <c r="L112"/>
-      <c r="M112" s="15"/>
-      <c r="N112"/>
-      <c r="O112"/>
-      <c r="P112"/>
-      <c r="Q112"/>
-      <c r="R112"/>
-      <c r="S112" s="15"/>
-      <c r="T112" s="1"/>
-    </row>
-    <row r="113" spans="1:20" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K112" s="15"/>
+      <c r="L112" s="1"/>
+    </row>
+    <row r="113" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A113" s="6" t="s">
         <v>124</v>
       </c>
@@ -4720,11 +4165,11 @@
         <v>16</v>
       </c>
       <c r="G113" s="15"/>
-      <c r="M113" s="15"/>
-      <c r="S113" s="15"/>
-      <c r="T113" s="1"/>
-    </row>
-    <row r="114" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I113" s="15"/>
+      <c r="K113" s="15"/>
+      <c r="L113" s="1"/>
+    </row>
+    <row r="114" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>127</v>
       </c>
@@ -4740,44 +4185,17 @@
       <c r="E114" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F114" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G114" s="15"/>
-      <c r="H114" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M114" s="15"/>
-      <c r="N114" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S114" s="15"/>
-      <c r="T114" s="1"/>
-    </row>
-    <row r="115" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I114" s="15"/>
+      <c r="K114" s="15"/>
+      <c r="L114" s="1"/>
+    </row>
+    <row r="115" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>5</v>
@@ -4791,42 +4209,15 @@
       <c r="E115" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F115" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G115" s="15"/>
-      <c r="H115" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M115" s="15"/>
-      <c r="N115" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S115" s="15"/>
-      <c r="T115" s="1"/>
-    </row>
-    <row r="116" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I115" s="15"/>
+      <c r="K115" s="15"/>
+      <c r="L115" s="1"/>
+    </row>
+    <row r="116" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
         <v>130</v>
       </c>
@@ -4843,22 +4234,22 @@
         <v>0</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G116" s="15"/>
-      <c r="M116" s="15"/>
-      <c r="S116" s="15"/>
-      <c r="T116" s="1"/>
-    </row>
-    <row r="117" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="I116" s="15"/>
+      <c r="K116" s="15"/>
+      <c r="L116" s="1"/>
+    </row>
+    <row r="117" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D117" s="2" t="b">
         <v>1</v>
@@ -4868,64 +4259,40 @@
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="I117" s="2" t="s">
-        <v>326</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="I117" s="15"/>
       <c r="J117" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="L117" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="M117" s="15"/>
-      <c r="N117" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="O117" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="P117" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q117" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R117" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S117" s="15"/>
-      <c r="T117" s="1"/>
-    </row>
-    <row r="118" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+        <v>316</v>
+      </c>
+      <c r="K117" s="15"/>
+      <c r="L117" s="1"/>
+    </row>
+    <row r="118" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C118" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F118" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D118" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E118" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="G118" s="15"/>
-      <c r="M118" s="15"/>
-      <c r="S118" s="15"/>
-      <c r="T118" s="1"/>
-    </row>
-    <row r="119" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="I118" s="15"/>
+      <c r="K118" s="15"/>
+      <c r="L118" s="1"/>
+    </row>
+    <row r="119" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>132</v>
       </c>
@@ -4942,78 +4309,78 @@
         <v>0</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G119" s="15"/>
-      <c r="M119" s="15"/>
-      <c r="S119" s="15"/>
-      <c r="T119" s="1"/>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T120" s="24"/>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T121" s="24"/>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T122" s="24"/>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T123" s="24"/>
-    </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T124" s="24"/>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T125" s="24"/>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T126" s="24"/>
-    </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T127" s="24"/>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="T128" s="24"/>
-    </row>
-    <row r="129" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T129" s="24"/>
-    </row>
-    <row r="130" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T130" s="24"/>
-    </row>
-    <row r="131" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T131" s="24"/>
-    </row>
-    <row r="132" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T132" s="24"/>
-    </row>
-    <row r="133" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T133" s="24"/>
-    </row>
-    <row r="134" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T134" s="24"/>
-    </row>
-    <row r="135" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T135" s="24"/>
-    </row>
-    <row r="136" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T136" s="24"/>
-    </row>
-    <row r="137" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T137" s="24"/>
-    </row>
-    <row r="138" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T138" s="24"/>
-    </row>
-    <row r="139" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T139" s="24"/>
-    </row>
-    <row r="140" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T140" s="24"/>
-    </row>
-    <row r="141" spans="20:20" x14ac:dyDescent="0.4">
-      <c r="T141" s="24"/>
+      <c r="I119" s="15"/>
+      <c r="K119" s="15"/>
+      <c r="L119" s="1"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L120" s="24"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L121" s="24"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L122" s="24"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L123" s="24"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L124" s="24"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L125" s="24"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L126" s="24"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L127" s="24"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L128" s="24"/>
+    </row>
+    <row r="129" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L129" s="24"/>
+    </row>
+    <row r="130" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L130" s="24"/>
+    </row>
+    <row r="131" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L131" s="24"/>
+    </row>
+    <row r="132" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L132" s="24"/>
+    </row>
+    <row r="133" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L133" s="24"/>
+    </row>
+    <row r="134" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L134" s="24"/>
+    </row>
+    <row r="135" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L135" s="24"/>
+    </row>
+    <row r="136" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L136" s="24"/>
+    </row>
+    <row r="137" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L137" s="24"/>
+    </row>
+    <row r="138" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L138" s="24"/>
+    </row>
+    <row r="139" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L139" s="24"/>
+    </row>
+    <row r="140" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L140" s="24"/>
+    </row>
+    <row r="141" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L141" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5050,48 +4417,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
IHW: aanpassingen aan weergave catalogus
Zie #680

Improvement
</commit_message>
<xml_diff>
--- a/src/main/resources/input/IHW/props/IHW.xlsx
+++ b/src/main/resources/input/IHW/props/IHW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\IHW\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2845AE-B8C2-4DE9-982D-E6C2FF528DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947AD4A6-D90E-4F9F-B735-8671F57A08E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IHW" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="319">
   <si>
     <t>Name</t>
   </si>
@@ -980,6 +980,9 @@
   </si>
   <si>
     <t>LOGICAL: uitgebreid</t>
+  </si>
+  <si>
+    <t>includemodelinfo</t>
   </si>
 </sst>
 </file>
@@ -1477,13 +1480,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L140"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E44" sqref="A44:XFD44"/>
+      <selection pane="bottomRight" activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2969,24 +2972,21 @@
       <c r="K63" s="15"/>
       <c r="L63" s="24"/>
     </row>
-    <row r="64" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D64" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>215</v>
+    <row r="64" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G64" s="15"/>
       <c r="I64" s="15"/>
@@ -2994,62 +2994,62 @@
       <c r="L64" s="24"/>
     </row>
     <row r="65" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>258</v>
-      </c>
-      <c r="B65" t="s">
-        <v>78</v>
-      </c>
-      <c r="C65" t="s">
-        <v>259</v>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>223</v>
+      <c r="A65" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="G65" s="15"/>
       <c r="I65" s="15"/>
       <c r="K65" s="15"/>
       <c r="L65" s="24"/>
     </row>
-    <row r="66" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>206</v>
+    <row r="66" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s">
+        <v>259</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>223</v>
       </c>
       <c r="G66" s="15"/>
       <c r="I66" s="15"/>
       <c r="K66" s="15"/>
       <c r="L66" s="24"/>
     </row>
-    <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
@@ -3058,31 +3058,31 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>273</v>
+        <v>206</v>
       </c>
       <c r="G67" s="15"/>
       <c r="I67" s="15"/>
       <c r="K67" s="15"/>
       <c r="L67" s="24"/>
     </row>
-    <row r="68" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
       <c r="G68" s="15"/>
       <c r="I68" s="15"/>
@@ -3091,13 +3091,13 @@
     </row>
     <row r="69" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>250</v>
+        <v>188</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>252</v>
+        <v>190</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
@@ -3106,52 +3106,52 @@
         <v>1</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="G69" s="15"/>
       <c r="I69" s="15"/>
       <c r="K69" s="15"/>
       <c r="L69" s="24"/>
     </row>
-    <row r="70" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>69</v>
+        <v>250</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>70</v>
+        <v>252</v>
       </c>
       <c r="D70" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="G70" s="15"/>
       <c r="I70" s="15"/>
       <c r="K70" s="15"/>
       <c r="L70" s="24"/>
     </row>
-    <row r="71" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>301</v>
+        <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>302</v>
+        <v>70</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>303</v>
+        <v>0</v>
       </c>
       <c r="G71" s="15"/>
       <c r="I71" s="15"/>
@@ -3160,13 +3160,13 @@
     </row>
     <row r="72" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D72" s="2" t="b">
         <v>0</v>
@@ -3175,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="G72" s="15"/>
       <c r="I72" s="15"/>
@@ -3184,13 +3184,13 @@
     </row>
     <row r="73" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
@@ -3198,26 +3198,23 @@
       <c r="E73" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F73" s="2" t="s">
+        <v>310</v>
+      </c>
       <c r="G73" s="15"/>
-      <c r="H73" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="I73" s="15"/>
-      <c r="J73" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="K73" s="15"/>
       <c r="L73" s="24"/>
     </row>
     <row r="74" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3226,19 +3223,25 @@
         <v>1</v>
       </c>
       <c r="G74" s="15"/>
+      <c r="H74" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="I74" s="15"/>
+      <c r="J74" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="K74" s="15"/>
       <c r="L74" s="24"/>
     </row>
     <row r="75" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>191</v>
+        <v>308</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3251,288 +3254,285 @@
       <c r="K75" s="15"/>
       <c r="L75" s="24"/>
     </row>
-    <row r="76" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>4</v>
+    <row r="76" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G76" s="15"/>
       <c r="I76" s="15"/>
       <c r="K76" s="15"/>
       <c r="L76" s="24"/>
     </row>
-    <row r="77" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="B77" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="D77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="2" t="s">
+    <row r="77" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G77" s="15"/>
       <c r="I77" s="15"/>
       <c r="K77" s="15"/>
-      <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>226</v>
+      <c r="L77" s="24"/>
+    </row>
+    <row r="78" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>293</v>
       </c>
       <c r="D78" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G78" s="15"/>
       <c r="I78" s="15"/>
       <c r="K78" s="15"/>
-      <c r="L78" s="24"/>
+      <c r="L78" s="1"/>
     </row>
     <row r="79" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>73</v>
+        <v>214</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>74</v>
+        <v>226</v>
       </c>
       <c r="D79" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G79" s="15"/>
       <c r="I79" s="15"/>
       <c r="K79" s="15"/>
       <c r="L79" s="24"/>
     </row>
-    <row r="80" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D80" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G80" s="15"/>
       <c r="I80" s="15"/>
       <c r="K80" s="15"/>
       <c r="L80" s="24"/>
     </row>
-    <row r="81" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D81" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="G81" s="15"/>
       <c r="I81" s="15"/>
       <c r="K81" s="15"/>
       <c r="L81" s="24"/>
     </row>
-    <row r="82" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D82" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>270</v>
+    <row r="82" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="G82" s="15"/>
       <c r="I82" s="15"/>
       <c r="K82" s="15"/>
       <c r="L82" s="24"/>
     </row>
-    <row r="83" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>19</v>
+    <row r="83" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="G83" s="15"/>
       <c r="I83" s="15"/>
       <c r="K83" s="15"/>
       <c r="L83" s="24"/>
     </row>
-    <row r="84" spans="1:12" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A84" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D84" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>207</v>
+    <row r="84" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G84" s="15"/>
       <c r="I84" s="15"/>
       <c r="K84" s="15"/>
       <c r="L84" s="24"/>
     </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>0</v>
+    <row r="85" spans="1:12" s="6" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A85" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="G85" s="15"/>
-      <c r="H85" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="I85" s="15"/>
-      <c r="J85" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="K85" s="15"/>
       <c r="L85" s="24"/>
     </row>
     <row r="86" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="G86" s="15"/>
+      <c r="H86" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="I86" s="15"/>
+      <c r="J86" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="K86" s="15"/>
       <c r="L86" s="24"/>
     </row>
-    <row r="87" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D87" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>89</v>
+    <row r="87" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G87" s="15"/>
       <c r="I87" s="15"/>
@@ -3541,22 +3541,22 @@
     </row>
     <row r="88" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="6" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="D88" s="6" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="G88" s="15"/>
       <c r="I88" s="15"/>
@@ -3564,69 +3564,73 @@
       <c r="L88" s="24"/>
     </row>
     <row r="89" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="20" t="s">
+      <c r="A89" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D89" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="24"/>
+    </row>
+    <row r="90" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="B89" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="20" t="s">
+      <c r="B90" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="D89" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="20" t="s">
+      <c r="D90" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G89" s="15"/>
-      <c r="H89" s="20"/>
-      <c r="I89" s="21"/>
-      <c r="J89" s="20"/>
-      <c r="K89" s="21"/>
-      <c r="L89" s="25"/>
-    </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
+      <c r="G90" s="15"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="20"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="25"/>
+    </row>
+    <row r="91" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" s="2" t="s">
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G90" s="15"/>
-      <c r="I90" s="15"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="24"/>
-    </row>
-    <row r="91" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G91" s="15"/>
       <c r="I91" s="15"/>
@@ -3635,22 +3639,18 @@
     </row>
     <row r="92" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>148</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
       <c r="D92" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G92" s="15"/>
       <c r="I92" s="15"/>
@@ -3659,46 +3659,46 @@
     </row>
     <row r="93" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="D93" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>264</v>
+        <v>4</v>
       </c>
       <c r="G93" s="15"/>
       <c r="I93" s="15"/>
       <c r="K93" s="15"/>
       <c r="L93" s="24"/>
     </row>
-    <row r="94" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>197</v>
+        <v>95</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>198</v>
+        <v>10</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>199</v>
+        <v>96</v>
       </c>
       <c r="D94" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="G94" s="15"/>
       <c r="I94" s="15"/>
@@ -3707,13 +3707,13 @@
     </row>
     <row r="95" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>244</v>
+        <v>197</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>245</v>
+        <v>198</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>246</v>
+        <v>199</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
@@ -3721,115 +3721,115 @@
       <c r="E95" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="5" t="s">
-        <v>247</v>
+      <c r="F95" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="G95" s="15"/>
       <c r="I95" s="15"/>
       <c r="K95" s="15"/>
       <c r="L95" s="24"/>
     </row>
-    <row r="96" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+        <v>244</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>246</v>
+      </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>270</v>
+      <c r="F96" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="G96" s="15"/>
       <c r="I96" s="15"/>
       <c r="K96" s="15"/>
       <c r="L96" s="24"/>
     </row>
-    <row r="97" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>98</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
       <c r="D97" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="G97" s="15"/>
       <c r="I97" s="15"/>
       <c r="K97" s="15"/>
       <c r="L97" s="24"/>
     </row>
-    <row r="98" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
-        <v>276</v>
-      </c>
-      <c r="B98" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" t="s">
-        <v>277</v>
-      </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" t="s">
-        <v>270</v>
+    <row r="98" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G98" s="15"/>
       <c r="I98" s="15"/>
       <c r="K98" s="15"/>
-      <c r="L98" s="1"/>
-    </row>
-    <row r="99" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>208</v>
+      <c r="L98" s="24"/>
+    </row>
+    <row r="99" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>276</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" t="s">
+        <v>277</v>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>270</v>
       </c>
       <c r="G99" s="15"/>
       <c r="I99" s="15"/>
       <c r="K99" s="15"/>
-      <c r="L99" s="24"/>
+      <c r="L99" s="1"/>
     </row>
     <row r="100" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D100" s="2" t="b">
         <v>0</v>
@@ -3837,29 +3837,32 @@
       <c r="E100" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F100" s="2" t="s">
-        <v>16</v>
+      <c r="F100" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="G100" s="15"/>
       <c r="I100" s="15"/>
       <c r="K100" s="15"/>
       <c r="L100" s="24"/>
     </row>
-    <row r="101" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>201</v>
+        <v>102</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E101" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G101" s="15"/>
       <c r="I101" s="15"/>
@@ -3868,37 +3871,34 @@
     </row>
     <row r="102" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>103</v>
+        <v>200</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>106</v>
+        <v>201</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="G102" s="15"/>
       <c r="I102" s="15"/>
       <c r="K102" s="15"/>
       <c r="L102" s="24"/>
     </row>
-    <row r="103" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D103" s="2" t="b">
         <v>1</v>
@@ -3906,50 +3906,50 @@
       <c r="E103" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F103" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="G103" s="15"/>
-      <c r="H103" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="I103" s="15"/>
-      <c r="J103" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="K103" s="15"/>
       <c r="L103" s="24"/>
     </row>
-    <row r="104" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D104" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>215</v>
+    <row r="104" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G104" s="15"/>
+      <c r="H104" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="I104" s="15"/>
+      <c r="J104" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="K104" s="15"/>
       <c r="L104" s="24"/>
     </row>
     <row r="105" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D105" s="6" t="b">
         <v>1</v>
@@ -3967,46 +3967,46 @@
     </row>
     <row r="106" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D106" s="6" t="b">
         <v>1</v>
       </c>
       <c r="E106" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="G106" s="15"/>
       <c r="I106" s="15"/>
       <c r="K106" s="15"/>
       <c r="L106" s="24"/>
     </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>4</v>
+    <row r="107" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D107" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G107" s="15"/>
       <c r="I107" s="15"/>
@@ -4015,16 +4015,16 @@
     </row>
     <row r="108" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D108" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108" s="2" t="b">
         <v>1</v>
@@ -4039,16 +4039,16 @@
     </row>
     <row r="109" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D109" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" s="2" t="b">
         <v>1</v>
@@ -4061,15 +4061,15 @@
       <c r="K109" s="15"/>
       <c r="L109" s="24"/>
     </row>
-    <row r="110" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D110" s="2" t="b">
         <v>0</v>
@@ -4081,79 +4081,79 @@
         <v>4</v>
       </c>
       <c r="G110" s="15"/>
-      <c r="H110"/>
       <c r="I110" s="15"/>
       <c r="K110" s="15"/>
       <c r="L110" s="24"/>
     </row>
-    <row r="111" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>278</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D111" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
+    <row r="111" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111"/>
       <c r="I111" s="15"/>
-      <c r="J111"/>
       <c r="K111" s="15"/>
-      <c r="L111" s="1"/>
-    </row>
-    <row r="112" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D112" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>16</v>
+      <c r="L111" s="24"/>
+    </row>
+    <row r="112" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>278</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>279</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>4</v>
       </c>
       <c r="G112" s="15"/>
+      <c r="H112"/>
       <c r="I112" s="15"/>
+      <c r="J112"/>
       <c r="K112" s="15"/>
       <c r="L112" s="1"/>
     </row>
-    <row r="113" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>4</v>
+    <row r="113" spans="1:12" s="6" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A113" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D113" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G113" s="15"/>
       <c r="I113" s="15"/>
@@ -4162,13 +4162,13 @@
     </row>
     <row r="114" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>235</v>
+        <v>124</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D114" s="2" t="b">
         <v>1</v>
@@ -4186,22 +4186,22 @@
     </row>
     <row r="115" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D115" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E115" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>270</v>
+        <v>4</v>
       </c>
       <c r="G115" s="15"/>
       <c r="I115" s="15"/>
@@ -4210,40 +4210,37 @@
     </row>
     <row r="116" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>290</v>
+        <v>127</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>291</v>
+        <v>128</v>
       </c>
       <c r="D116" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E116" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="G116" s="15"/>
-      <c r="H116" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="I116" s="15"/>
-      <c r="J116" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="K116" s="15"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>254</v>
+        <v>291</v>
       </c>
       <c r="D117" s="2" t="b">
         <v>1</v>
@@ -4251,40 +4248,64 @@
       <c r="E117" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="G117" s="15"/>
+      <c r="H117" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="I117" s="15"/>
+      <c r="J117" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="K117" s="15"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>129</v>
+        <v>253</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>131</v>
+        <v>254</v>
       </c>
       <c r="D118" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>223</v>
+        <v>255</v>
       </c>
       <c r="G118" s="15"/>
       <c r="I118" s="15"/>
       <c r="K118" s="15"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L119" s="24"/>
+    <row r="119" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A119" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G119" s="15"/>
+      <c r="I119" s="15"/>
+      <c r="K119" s="15"/>
+      <c r="L119" s="1"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.4">
       <c r="L120" s="24"/>
@@ -4348,6 +4369,9 @@
     </row>
     <row r="140" spans="12:12" x14ac:dyDescent="0.4">
       <c r="L140" s="24"/>
+    </row>
+    <row r="141" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="L141" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>